<commit_message>
changed subtitles and timetable
</commit_message>
<xml_diff>
--- a/TerminplanungP2.xlsx
+++ b/TerminplanungP2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\EIT\FS19\pro2E\Team 5\P2Pflichtenheft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lkrummenacher/Documents/GitHub/P2Pflichtenheft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C206809-6DA5-464D-8893-9F7C1A9A7A30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F2B0DB-6B84-434B-A481-0B3840D460E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Terminplanung" sheetId="1" r:id="rId1"/>
     <sheet name="Projektbudget" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Terminplanung!$A$62:$W$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Terminplanung!$A$63:$W$89</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Terminplanung!$A:$A,Terminplanung!$2:$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="166">
   <si>
     <t>Meilensteine</t>
   </si>
@@ -540,6 +540,18 @@
   </si>
   <si>
     <t>3.3.2 Bedienungsanleitung erstellen</t>
+  </si>
+  <si>
+    <t>3.3.3 Software mit Testkonzept validieren</t>
+  </si>
+  <si>
+    <t>4.2.1 Berechnungen für Javacode anpassen</t>
+  </si>
+  <si>
+    <t>4.2.3 Auswertung der Daten von der Software</t>
+  </si>
+  <si>
+    <t>4.2.2 Validieren der Berechnungen im Code</t>
   </si>
 </sst>
 </file>
@@ -686,7 +698,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -804,6 +816,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1049,7 +1073,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1413,18 +1437,39 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1434,27 +1479,6 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1484,6 +1508,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2193,55 +2231,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR91"/>
+  <dimension ref="A1:AR92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="118" zoomScaleNormal="90" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="U82" sqref="U82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="45.69921875" style="61" customWidth="1"/>
-    <col min="2" max="2" width="4.69921875" style="129" customWidth="1"/>
-    <col min="3" max="23" width="6.69921875" style="61" customWidth="1"/>
-    <col min="24" max="16384" width="10.796875" style="61"/>
+    <col min="1" max="1" width="45.6640625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="129" customWidth="1"/>
+    <col min="3" max="23" width="6.6640625" style="61" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="170" t="s">
+    <row r="1" spans="1:23" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="165" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="156"/>
-      <c r="B2" s="170"/>
-      <c r="C2" s="165">
+      <c r="B2" s="165"/>
+      <c r="C2" s="158">
         <v>2019</v>
       </c>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
-      <c r="Q2" s="166"/>
-      <c r="R2" s="166"/>
-      <c r="S2" s="166"/>
-      <c r="T2" s="166"/>
-      <c r="U2" s="166"/>
-      <c r="V2" s="166"/>
-      <c r="W2" s="167"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="159"/>
+      <c r="Q2" s="159"/>
+      <c r="R2" s="159"/>
+      <c r="S2" s="159"/>
+      <c r="T2" s="159"/>
+      <c r="U2" s="159"/>
+      <c r="V2" s="159"/>
+      <c r="W2" s="160"/>
+    </row>
+    <row r="3" spans="1:23" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="156"/>
-      <c r="B3" s="170"/>
+      <c r="B3" s="165"/>
       <c r="C3" s="63" t="s">
         <v>87</v>
       </c>
@@ -2275,13 +2313,13 @@
       <c r="M3" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="N3" s="165" t="s">
+      <c r="N3" s="158" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="166"/>
-      <c r="P3" s="166"/>
-      <c r="Q3" s="166"/>
-      <c r="R3" s="166"/>
+      <c r="O3" s="159"/>
+      <c r="P3" s="159"/>
+      <c r="Q3" s="159"/>
+      <c r="R3" s="159"/>
       <c r="S3" s="64" t="s">
         <v>98</v>
       </c>
@@ -2298,9 +2336,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" s="156"/>
-      <c r="B4" s="170"/>
+      <c r="B4" s="165"/>
       <c r="C4" s="63">
         <v>18.02</v>
       </c>
@@ -2365,14 +2403,14 @@
         <v>10.06</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="170"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="165"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A6" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="170"/>
+      <c r="B6" s="165"/>
       <c r="C6" s="122"/>
       <c r="D6" s="122"/>
       <c r="E6" s="122"/>
@@ -2395,32 +2433,32 @@
       <c r="V6" s="122"/>
       <c r="W6" s="122"/>
     </row>
-    <row r="7" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="157"/>
-      <c r="B7" s="157"/>
-      <c r="C7" s="157"/>
-      <c r="D7" s="157"/>
-      <c r="E7" s="157"/>
-      <c r="F7" s="157"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="157"/>
-      <c r="I7" s="157"/>
-      <c r="J7" s="157"/>
-      <c r="K7" s="157"/>
-      <c r="L7" s="157"/>
-      <c r="M7" s="157"/>
-      <c r="N7" s="157"/>
-      <c r="O7" s="157"/>
-      <c r="P7" s="157"/>
-      <c r="Q7" s="157"/>
-      <c r="R7" s="157"/>
-      <c r="S7" s="157"/>
-      <c r="T7" s="157"/>
-      <c r="U7" s="157"/>
-      <c r="V7" s="157"/>
-      <c r="W7" s="157"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="166"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
+      <c r="G7" s="166"/>
+      <c r="H7" s="166"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
+      <c r="L7" s="166"/>
+      <c r="M7" s="166"/>
+      <c r="N7" s="166"/>
+      <c r="O7" s="166"/>
+      <c r="P7" s="166"/>
+      <c r="Q7" s="166"/>
+      <c r="R7" s="166"/>
+      <c r="S7" s="166"/>
+      <c r="T7" s="166"/>
+      <c r="U7" s="166"/>
+      <c r="V7" s="166"/>
+      <c r="W7" s="166"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="66" t="s">
         <v>1</v>
       </c>
@@ -2449,7 +2487,7 @@
       <c r="V8" s="63"/>
       <c r="W8" s="63"/>
     </row>
-    <row r="9" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9" s="66" t="s">
         <v>103</v>
       </c>
@@ -2478,7 +2516,7 @@
       <c r="V9" s="63"/>
       <c r="W9" s="63"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" s="66" t="s">
         <v>106</v>
       </c>
@@ -2507,7 +2545,7 @@
       <c r="V10" s="63"/>
       <c r="W10" s="63"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" s="70" t="s">
         <v>104</v>
       </c>
@@ -2536,7 +2574,7 @@
       <c r="V11" s="63"/>
       <c r="W11" s="63"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" s="70" t="s">
         <v>105</v>
       </c>
@@ -2565,7 +2603,7 @@
       <c r="V12" s="63"/>
       <c r="W12" s="63"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13" s="71" t="s">
         <v>107</v>
       </c>
@@ -2594,7 +2632,7 @@
       <c r="V13" s="63"/>
       <c r="W13" s="63"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14" s="70" t="s">
         <v>108</v>
       </c>
@@ -2622,7 +2660,7 @@
       <c r="V14" s="63"/>
       <c r="W14" s="63"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" s="70" t="s">
         <v>109</v>
       </c>
@@ -2653,7 +2691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" s="66" t="s">
         <v>110</v>
       </c>
@@ -2682,7 +2720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17" s="70" t="s">
         <v>111</v>
       </c>
@@ -2711,7 +2749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A18" s="61" t="s">
         <v>86</v>
       </c>
@@ -2737,63 +2775,63 @@
       <c r="V18" s="63"/>
       <c r="W18" s="63"/>
     </row>
-    <row r="19" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="158"/>
-      <c r="B19" s="158"/>
-      <c r="C19" s="158"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
-      <c r="K19" s="158"/>
-      <c r="L19" s="158"/>
-      <c r="M19" s="158"/>
-      <c r="N19" s="158"/>
-      <c r="O19" s="158"/>
-      <c r="P19" s="158"/>
-      <c r="Q19" s="158"/>
-      <c r="R19" s="158"/>
-      <c r="S19" s="158"/>
-      <c r="T19" s="158"/>
-      <c r="U19" s="158"/>
-      <c r="V19" s="158"/>
-      <c r="W19" s="158"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="167"/>
+      <c r="B19" s="167"/>
+      <c r="C19" s="167"/>
+      <c r="D19" s="167"/>
+      <c r="E19" s="167"/>
+      <c r="F19" s="167"/>
+      <c r="G19" s="167"/>
+      <c r="H19" s="167"/>
+      <c r="I19" s="167"/>
+      <c r="J19" s="167"/>
+      <c r="K19" s="167"/>
+      <c r="L19" s="167"/>
+      <c r="M19" s="167"/>
+      <c r="N19" s="167"/>
+      <c r="O19" s="167"/>
+      <c r="P19" s="167"/>
+      <c r="Q19" s="167"/>
+      <c r="R19" s="167"/>
+      <c r="S19" s="167"/>
+      <c r="T19" s="167"/>
+      <c r="U19" s="167"/>
+      <c r="V19" s="167"/>
+      <c r="W19" s="167"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A20" s="121" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="135"/>
     </row>
-    <row r="21" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="157"/>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="157"/>
-      <c r="L21" s="157"/>
-      <c r="M21" s="157"/>
-      <c r="N21" s="157"/>
-      <c r="O21" s="157"/>
-      <c r="P21" s="157"/>
-      <c r="Q21" s="157"/>
-      <c r="R21" s="157"/>
-      <c r="S21" s="157"/>
-      <c r="T21" s="157"/>
-      <c r="U21" s="157"/>
-      <c r="V21" s="157"/>
-      <c r="W21" s="157"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="6" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="166"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="166"/>
+      <c r="D21" s="166"/>
+      <c r="E21" s="166"/>
+      <c r="F21" s="166"/>
+      <c r="G21" s="166"/>
+      <c r="H21" s="166"/>
+      <c r="I21" s="166"/>
+      <c r="J21" s="166"/>
+      <c r="K21" s="166"/>
+      <c r="L21" s="166"/>
+      <c r="M21" s="166"/>
+      <c r="N21" s="166"/>
+      <c r="O21" s="166"/>
+      <c r="P21" s="166"/>
+      <c r="Q21" s="166"/>
+      <c r="R21" s="166"/>
+      <c r="S21" s="166"/>
+      <c r="T21" s="166"/>
+      <c r="U21" s="166"/>
+      <c r="V21" s="166"/>
+      <c r="W21" s="166"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A22" s="100" t="s">
         <v>5</v>
       </c>
@@ -2820,7 +2858,7 @@
       <c r="V22" s="102"/>
       <c r="W22" s="103"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A23" s="72" t="s">
         <v>117</v>
       </c>
@@ -2849,7 +2887,7 @@
       <c r="V23" s="104"/>
       <c r="W23" s="104"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A24" s="72" t="s">
         <v>137</v>
       </c>
@@ -2878,7 +2916,7 @@
       <c r="V24" s="66"/>
       <c r="W24" s="66"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A25" s="83" t="s">
         <v>138</v>
       </c>
@@ -2905,7 +2943,7 @@
       <c r="V25" s="66"/>
       <c r="W25" s="66"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A26" s="83" t="s">
         <v>139</v>
       </c>
@@ -2932,7 +2970,7 @@
       <c r="V26" s="66"/>
       <c r="W26" s="66"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A27" s="83" t="s">
         <v>140</v>
       </c>
@@ -2959,7 +2997,7 @@
       <c r="V27" s="66"/>
       <c r="W27" s="66"/>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A28" s="72" t="s">
         <v>121</v>
       </c>
@@ -2988,7 +3026,7 @@
       <c r="V28" s="66"/>
       <c r="W28" s="66"/>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A29" s="83" t="s">
         <v>141</v>
       </c>
@@ -3015,7 +3053,7 @@
       <c r="V29" s="66"/>
       <c r="W29" s="66"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="87" t="s">
         <v>113</v>
       </c>
@@ -3044,7 +3082,7 @@
       <c r="V30" s="66"/>
       <c r="W30" s="66"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="87" t="s">
         <v>114</v>
       </c>
@@ -3073,7 +3111,7 @@
       <c r="V31" s="66"/>
       <c r="W31" s="66"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="87" t="s">
         <v>115</v>
       </c>
@@ -3102,7 +3140,7 @@
       <c r="V32" s="66"/>
       <c r="W32" s="66"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="87" t="s">
         <v>116</v>
       </c>
@@ -3131,7 +3169,7 @@
       <c r="V33" s="107"/>
       <c r="W33" s="107"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="87" t="s">
         <v>142</v>
       </c>
@@ -3160,7 +3198,7 @@
       <c r="V34" s="107"/>
       <c r="W34" s="107"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="75" t="s">
         <v>143</v>
       </c>
@@ -3187,7 +3225,7 @@
       <c r="V35" s="107"/>
       <c r="W35" s="107"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="75" t="s">
         <v>144</v>
       </c>
@@ -3214,7 +3252,7 @@
       <c r="V36" s="107"/>
       <c r="W36" s="107"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A37" s="72" t="s">
         <v>122</v>
       </c>
@@ -3241,32 +3279,32 @@
       <c r="V37" s="106"/>
       <c r="W37" s="106"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" s="159"/>
-      <c r="B38" s="160"/>
-      <c r="C38" s="160"/>
-      <c r="D38" s="160"/>
-      <c r="E38" s="160"/>
-      <c r="F38" s="160"/>
-      <c r="G38" s="160"/>
-      <c r="H38" s="160"/>
-      <c r="I38" s="160"/>
-      <c r="J38" s="160"/>
-      <c r="K38" s="160"/>
-      <c r="L38" s="160"/>
-      <c r="M38" s="160"/>
-      <c r="N38" s="160"/>
-      <c r="O38" s="160"/>
-      <c r="P38" s="160"/>
-      <c r="Q38" s="160"/>
-      <c r="R38" s="160"/>
-      <c r="S38" s="160"/>
-      <c r="T38" s="160"/>
-      <c r="U38" s="160"/>
-      <c r="V38" s="160"/>
-      <c r="W38" s="160"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A38" s="163"/>
+      <c r="B38" s="164"/>
+      <c r="C38" s="164"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
+      <c r="F38" s="164"/>
+      <c r="G38" s="164"/>
+      <c r="H38" s="164"/>
+      <c r="I38" s="164"/>
+      <c r="J38" s="164"/>
+      <c r="K38" s="164"/>
+      <c r="L38" s="164"/>
+      <c r="M38" s="164"/>
+      <c r="N38" s="164"/>
+      <c r="O38" s="164"/>
+      <c r="P38" s="164"/>
+      <c r="Q38" s="164"/>
+      <c r="R38" s="164"/>
+      <c r="S38" s="164"/>
+      <c r="T38" s="164"/>
+      <c r="U38" s="164"/>
+      <c r="V38" s="164"/>
+      <c r="W38" s="164"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A39" s="88" t="s">
         <v>11</v>
       </c>
@@ -3293,7 +3331,7 @@
       <c r="V39" s="91"/>
       <c r="W39" s="91"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A40" s="77" t="s">
         <v>119</v>
       </c>
@@ -3322,7 +3360,7 @@
       <c r="V40" s="79"/>
       <c r="W40" s="79"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A41" s="134" t="s">
         <v>131</v>
       </c>
@@ -3349,7 +3387,7 @@
       <c r="V41" s="79"/>
       <c r="W41" s="79"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A42" s="134" t="s">
         <v>151</v>
       </c>
@@ -3376,7 +3414,7 @@
       <c r="V42" s="79"/>
       <c r="W42" s="79"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A43" s="134" t="s">
         <v>152</v>
       </c>
@@ -3403,7 +3441,7 @@
       <c r="V43" s="79"/>
       <c r="W43" s="79"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A44" s="77"/>
       <c r="B44" s="142"/>
       <c r="C44" s="78"/>
@@ -3428,7 +3466,7 @@
       <c r="V44" s="79"/>
       <c r="W44" s="79"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A45" s="72" t="s">
         <v>120</v>
       </c>
@@ -3457,7 +3495,7 @@
       <c r="V45" s="66"/>
       <c r="W45" s="66"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A46" s="75" t="s">
         <v>149</v>
       </c>
@@ -3484,7 +3522,7 @@
       <c r="V46" s="66"/>
       <c r="W46" s="66"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A47" s="75" t="s">
         <v>158</v>
       </c>
@@ -3511,7 +3549,7 @@
       <c r="V47" s="66"/>
       <c r="W47" s="66"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="15" x14ac:dyDescent="0.15">
       <c r="A48" s="81" t="s">
         <v>150</v>
       </c>
@@ -3538,32 +3576,32 @@
       <c r="V48" s="66"/>
       <c r="W48" s="66"/>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A49" s="159"/>
-      <c r="B49" s="160"/>
-      <c r="C49" s="160"/>
-      <c r="D49" s="160"/>
-      <c r="E49" s="160"/>
-      <c r="F49" s="160"/>
-      <c r="G49" s="160"/>
-      <c r="H49" s="160"/>
-      <c r="I49" s="160"/>
-      <c r="J49" s="160"/>
-      <c r="K49" s="160"/>
-      <c r="L49" s="160"/>
-      <c r="M49" s="160"/>
-      <c r="N49" s="160"/>
-      <c r="O49" s="160"/>
-      <c r="P49" s="160"/>
-      <c r="Q49" s="160"/>
-      <c r="R49" s="160"/>
-      <c r="S49" s="160"/>
-      <c r="T49" s="160"/>
-      <c r="U49" s="160"/>
-      <c r="V49" s="160"/>
-      <c r="W49" s="160"/>
-    </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A49" s="163"/>
+      <c r="B49" s="164"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="164"/>
+      <c r="E49" s="164"/>
+      <c r="F49" s="164"/>
+      <c r="G49" s="164"/>
+      <c r="H49" s="164"/>
+      <c r="I49" s="164"/>
+      <c r="J49" s="164"/>
+      <c r="K49" s="164"/>
+      <c r="L49" s="164"/>
+      <c r="M49" s="164"/>
+      <c r="N49" s="164"/>
+      <c r="O49" s="164"/>
+      <c r="P49" s="164"/>
+      <c r="Q49" s="164"/>
+      <c r="R49" s="164"/>
+      <c r="S49" s="164"/>
+      <c r="T49" s="164"/>
+      <c r="U49" s="164"/>
+      <c r="V49" s="164"/>
+      <c r="W49" s="164"/>
+    </row>
+    <row r="50" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A50" s="94" t="s">
         <v>24</v>
       </c>
@@ -3590,7 +3628,7 @@
       <c r="V50" s="96"/>
       <c r="W50" s="96"/>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A51" s="72" t="s">
         <v>123</v>
       </c>
@@ -3619,7 +3657,7 @@
       <c r="V51" s="76"/>
       <c r="W51" s="76"/>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A52" s="83" t="s">
         <v>132</v>
       </c>
@@ -3646,7 +3684,7 @@
       <c r="V52" s="76"/>
       <c r="W52" s="76"/>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A53" s="83" t="s">
         <v>133</v>
       </c>
@@ -3673,7 +3711,7 @@
       <c r="V53" s="66"/>
       <c r="W53" s="66"/>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A54" s="83" t="s">
         <v>134</v>
       </c>
@@ -3700,7 +3738,7 @@
       <c r="V54" s="66"/>
       <c r="W54" s="66"/>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A55" s="72" t="s">
         <v>124</v>
       </c>
@@ -3729,7 +3767,7 @@
       <c r="V55" s="76"/>
       <c r="W55" s="76"/>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A56" s="83" t="s">
         <v>153</v>
       </c>
@@ -3739,9 +3777,9 @@
       <c r="E56" s="73"/>
       <c r="F56" s="76"/>
       <c r="G56" s="76"/>
-      <c r="H56" s="73"/>
-      <c r="I56" s="73"/>
-      <c r="J56" s="73"/>
+      <c r="H56" s="153"/>
+      <c r="I56" s="153"/>
+      <c r="J56" s="153"/>
       <c r="K56" s="76"/>
       <c r="L56" s="76"/>
       <c r="M56" s="76"/>
@@ -3756,7 +3794,7 @@
       <c r="V56" s="76"/>
       <c r="W56" s="76"/>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A57" s="83" t="s">
         <v>154</v>
       </c>
@@ -3767,9 +3805,9 @@
       <c r="F57" s="76"/>
       <c r="G57" s="76"/>
       <c r="H57" s="73"/>
-      <c r="I57" s="73"/>
-      <c r="J57" s="73"/>
-      <c r="K57" s="76"/>
+      <c r="I57" s="153"/>
+      <c r="J57" s="153"/>
+      <c r="K57" s="154"/>
       <c r="L57" s="76"/>
       <c r="M57" s="76"/>
       <c r="N57" s="125"/>
@@ -3783,7 +3821,7 @@
       <c r="V57" s="76"/>
       <c r="W57" s="76"/>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A58" s="83" t="s">
         <v>159</v>
       </c>
@@ -3795,9 +3833,9 @@
       <c r="G58" s="76"/>
       <c r="H58" s="73"/>
       <c r="I58" s="73"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="76"/>
-      <c r="L58" s="76"/>
+      <c r="J58" s="153"/>
+      <c r="K58" s="154"/>
+      <c r="L58" s="154"/>
       <c r="M58" s="66"/>
       <c r="N58" s="126"/>
       <c r="O58" s="127"/>
@@ -3810,7 +3848,7 @@
       <c r="V58" s="76"/>
       <c r="W58" s="76"/>
     </row>
-    <row r="59" spans="1:44" s="84" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:44" s="84" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A59" s="72" t="s">
         <v>125</v>
       </c>
@@ -3845,7 +3883,7 @@
       <c r="AB59" s="61"/>
       <c r="AC59" s="61"/>
     </row>
-    <row r="60" spans="1:44" s="84" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:44" s="84" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A60" s="83" t="s">
         <v>160</v>
       </c>
@@ -3878,7 +3916,7 @@
       <c r="AB60" s="61"/>
       <c r="AC60" s="61"/>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A61" s="83" t="s">
         <v>161</v>
       </c>
@@ -3892,8 +3930,8 @@
       <c r="I61" s="76"/>
       <c r="J61" s="76"/>
       <c r="K61" s="76"/>
-      <c r="L61" s="76"/>
-      <c r="M61" s="76"/>
+      <c r="L61" s="154"/>
+      <c r="M61" s="154"/>
       <c r="N61" s="125"/>
       <c r="O61" s="127"/>
       <c r="P61" s="127"/>
@@ -3905,116 +3943,116 @@
       <c r="V61" s="76"/>
       <c r="W61" s="76"/>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A62" s="159"/>
-      <c r="B62" s="160"/>
-      <c r="C62" s="160"/>
-      <c r="D62" s="160"/>
-      <c r="E62" s="160"/>
-      <c r="F62" s="160"/>
-      <c r="G62" s="160"/>
-      <c r="H62" s="160"/>
-      <c r="I62" s="160"/>
-      <c r="J62" s="160"/>
-      <c r="K62" s="160"/>
-      <c r="L62" s="160"/>
-      <c r="M62" s="160"/>
-      <c r="N62" s="160"/>
-      <c r="O62" s="160"/>
-      <c r="P62" s="160"/>
-      <c r="Q62" s="160"/>
-      <c r="R62" s="160"/>
-      <c r="S62" s="160"/>
-      <c r="T62" s="160"/>
-      <c r="U62" s="160"/>
-      <c r="V62" s="160"/>
-      <c r="W62" s="160"/>
-    </row>
-    <row r="63" spans="1:44" s="98" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="108" t="s">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A62" s="181" t="s">
+        <v>162</v>
+      </c>
+      <c r="B62" s="138"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="76"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="76"/>
+      <c r="G62" s="76"/>
+      <c r="H62" s="76"/>
+      <c r="I62" s="76"/>
+      <c r="J62" s="76"/>
+      <c r="K62" s="76"/>
+      <c r="L62" s="184"/>
+      <c r="M62" s="184"/>
+      <c r="N62" s="125"/>
+      <c r="O62" s="127"/>
+      <c r="P62" s="127"/>
+      <c r="Q62" s="127"/>
+      <c r="R62" s="127"/>
+      <c r="S62" s="182"/>
+      <c r="T62" s="183"/>
+      <c r="U62" s="76"/>
+      <c r="V62" s="76"/>
+      <c r="W62" s="76"/>
+    </row>
+    <row r="63" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A63" s="163"/>
+      <c r="B63" s="164"/>
+      <c r="C63" s="164"/>
+      <c r="D63" s="164"/>
+      <c r="E63" s="164"/>
+      <c r="F63" s="164"/>
+      <c r="G63" s="164"/>
+      <c r="H63" s="164"/>
+      <c r="I63" s="164"/>
+      <c r="J63" s="164"/>
+      <c r="K63" s="164"/>
+      <c r="L63" s="164"/>
+      <c r="M63" s="164"/>
+      <c r="N63" s="164"/>
+      <c r="O63" s="164"/>
+      <c r="P63" s="164"/>
+      <c r="Q63" s="164"/>
+      <c r="R63" s="164"/>
+      <c r="S63" s="164"/>
+      <c r="T63" s="164"/>
+      <c r="U63" s="164"/>
+      <c r="V63" s="164"/>
+      <c r="W63" s="164"/>
+    </row>
+    <row r="64" spans="1:44" s="98" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="B63" s="146"/>
-      <c r="C63" s="109"/>
-      <c r="D63" s="109"/>
-      <c r="E63" s="109"/>
-      <c r="F63" s="110"/>
-      <c r="G63" s="110"/>
-      <c r="H63" s="110"/>
-      <c r="I63" s="110"/>
-      <c r="J63" s="110"/>
-      <c r="K63" s="110"/>
-      <c r="L63" s="110"/>
-      <c r="M63" s="110"/>
-      <c r="N63" s="110"/>
-      <c r="O63" s="110"/>
-      <c r="P63" s="110"/>
-      <c r="Q63" s="111"/>
-      <c r="R63" s="111"/>
-      <c r="S63" s="111"/>
-      <c r="T63" s="111"/>
-      <c r="U63" s="111"/>
-      <c r="V63" s="110"/>
-      <c r="W63" s="110"/>
-      <c r="X63" s="61"/>
-      <c r="Y63" s="61"/>
-      <c r="Z63" s="61"/>
-      <c r="AA63" s="61"/>
-      <c r="AB63" s="61"/>
-      <c r="AC63" s="61"/>
-      <c r="AD63" s="61"/>
-      <c r="AE63" s="61"/>
-      <c r="AF63" s="61"/>
-      <c r="AG63" s="61"/>
-      <c r="AH63" s="61"/>
-      <c r="AI63" s="61"/>
-      <c r="AJ63" s="61"/>
-      <c r="AK63" s="61"/>
-      <c r="AL63" s="61"/>
-      <c r="AM63" s="61"/>
-      <c r="AN63" s="61"/>
-      <c r="AO63" s="61"/>
-      <c r="AP63" s="61"/>
-      <c r="AQ63" s="61"/>
-      <c r="AR63" s="61"/>
-    </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A64" s="72" t="s">
+      <c r="B64" s="146"/>
+      <c r="C64" s="109"/>
+      <c r="D64" s="109"/>
+      <c r="E64" s="109"/>
+      <c r="F64" s="110"/>
+      <c r="G64" s="110"/>
+      <c r="H64" s="110"/>
+      <c r="I64" s="110"/>
+      <c r="J64" s="110"/>
+      <c r="K64" s="110"/>
+      <c r="L64" s="110"/>
+      <c r="M64" s="110"/>
+      <c r="N64" s="110"/>
+      <c r="O64" s="110"/>
+      <c r="P64" s="110"/>
+      <c r="Q64" s="111"/>
+      <c r="R64" s="111"/>
+      <c r="S64" s="111"/>
+      <c r="T64" s="111"/>
+      <c r="U64" s="111"/>
+      <c r="V64" s="110"/>
+      <c r="W64" s="110"/>
+      <c r="X64" s="61"/>
+      <c r="Y64" s="61"/>
+      <c r="Z64" s="61"/>
+      <c r="AA64" s="61"/>
+      <c r="AB64" s="61"/>
+      <c r="AC64" s="61"/>
+      <c r="AD64" s="61"/>
+      <c r="AE64" s="61"/>
+      <c r="AF64" s="61"/>
+      <c r="AG64" s="61"/>
+      <c r="AH64" s="61"/>
+      <c r="AI64" s="61"/>
+      <c r="AJ64" s="61"/>
+      <c r="AK64" s="61"/>
+      <c r="AL64" s="61"/>
+      <c r="AM64" s="61"/>
+      <c r="AN64" s="61"/>
+      <c r="AO64" s="61"/>
+      <c r="AP64" s="61"/>
+      <c r="AQ64" s="61"/>
+      <c r="AR64" s="61"/>
+    </row>
+    <row r="65" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A65" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="142" t="s">
+      <c r="B65" s="142" t="s">
         <v>146</v>
       </c>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
-      <c r="G64" s="76"/>
-      <c r="H64" s="76"/>
-      <c r="I64" s="76"/>
-      <c r="J64" s="76"/>
-      <c r="K64" s="76"/>
-      <c r="L64" s="73"/>
-      <c r="M64" s="73"/>
-      <c r="N64" s="128"/>
-      <c r="O64" s="128"/>
-      <c r="P64" s="128"/>
-      <c r="Q64" s="128"/>
-      <c r="R64" s="128"/>
-      <c r="S64" s="73"/>
-      <c r="T64" s="73"/>
-      <c r="U64" s="76"/>
-      <c r="V64" s="76"/>
-      <c r="W64" s="76"/>
-    </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A65" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="B65" s="140"/>
-      <c r="C65" s="73"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="73"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
       <c r="F65" s="76"/>
       <c r="G65" s="76"/>
       <c r="H65" s="76"/>
@@ -4029,14 +4067,14 @@
       <c r="Q65" s="128"/>
       <c r="R65" s="128"/>
       <c r="S65" s="73"/>
-      <c r="T65" s="76"/>
+      <c r="T65" s="73"/>
       <c r="U65" s="76"/>
       <c r="V65" s="76"/>
       <c r="W65" s="76"/>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:44" ht="15" x14ac:dyDescent="0.15">
       <c r="A66" s="75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B66" s="140"/>
       <c r="C66" s="73"/>
@@ -4056,14 +4094,14 @@
       <c r="Q66" s="128"/>
       <c r="R66" s="128"/>
       <c r="S66" s="73"/>
-      <c r="T66" s="73"/>
+      <c r="T66" s="76"/>
       <c r="U66" s="76"/>
       <c r="V66" s="76"/>
       <c r="W66" s="76"/>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A67" s="155" t="s">
-        <v>157</v>
+    <row r="67" spans="1:44" ht="15" x14ac:dyDescent="0.15">
+      <c r="A67" s="75" t="s">
+        <v>156</v>
       </c>
       <c r="B67" s="140"/>
       <c r="C67" s="73"/>
@@ -4075,11 +4113,11 @@
       <c r="I67" s="76"/>
       <c r="J67" s="76"/>
       <c r="K67" s="76"/>
-      <c r="L67" s="76"/>
-      <c r="M67" s="76"/>
-      <c r="N67" s="125"/>
-      <c r="O67" s="127"/>
-      <c r="P67" s="127"/>
+      <c r="L67" s="73"/>
+      <c r="M67" s="73"/>
+      <c r="N67" s="128"/>
+      <c r="O67" s="128"/>
+      <c r="P67" s="128"/>
       <c r="Q67" s="128"/>
       <c r="R67" s="128"/>
       <c r="S67" s="73"/>
@@ -4088,13 +4126,11 @@
       <c r="V67" s="76"/>
       <c r="W67" s="76"/>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A68" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="138" t="s">
-        <v>147</v>
-      </c>
+    <row r="68" spans="1:44" ht="15" x14ac:dyDescent="0.15">
+      <c r="A68" s="155" t="s">
+        <v>157</v>
+      </c>
+      <c r="B68" s="140"/>
       <c r="C68" s="73"/>
       <c r="D68" s="73"/>
       <c r="E68" s="73"/>
@@ -4104,11 +4140,11 @@
       <c r="I68" s="76"/>
       <c r="J68" s="76"/>
       <c r="K68" s="76"/>
-      <c r="L68" s="73"/>
-      <c r="M68" s="73"/>
-      <c r="N68" s="128"/>
-      <c r="O68" s="128"/>
-      <c r="P68" s="128"/>
+      <c r="L68" s="76"/>
+      <c r="M68" s="76"/>
+      <c r="N68" s="125"/>
+      <c r="O68" s="127"/>
+      <c r="P68" s="127"/>
       <c r="Q68" s="128"/>
       <c r="R68" s="128"/>
       <c r="S68" s="73"/>
@@ -4117,9 +4153,13 @@
       <c r="V68" s="76"/>
       <c r="W68" s="76"/>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A69" s="75"/>
-      <c r="B69" s="140"/>
+    <row r="69" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A69" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="138" t="s">
+        <v>147</v>
+      </c>
       <c r="C69" s="73"/>
       <c r="D69" s="73"/>
       <c r="E69" s="73"/>
@@ -4129,21 +4169,23 @@
       <c r="I69" s="76"/>
       <c r="J69" s="76"/>
       <c r="K69" s="76"/>
-      <c r="L69" s="76"/>
-      <c r="M69" s="76"/>
+      <c r="L69" s="73"/>
+      <c r="M69" s="73"/>
       <c r="N69" s="128"/>
       <c r="O69" s="128"/>
       <c r="P69" s="128"/>
       <c r="Q69" s="128"/>
       <c r="R69" s="128"/>
       <c r="S69" s="73"/>
-      <c r="T69" s="76"/>
+      <c r="T69" s="73"/>
       <c r="U69" s="76"/>
       <c r="V69" s="76"/>
       <c r="W69" s="76"/>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A70" s="75"/>
+    <row r="70" spans="1:44" ht="15" x14ac:dyDescent="0.15">
+      <c r="A70" s="75" t="s">
+        <v>163</v>
+      </c>
       <c r="B70" s="140"/>
       <c r="C70" s="73"/>
       <c r="D70" s="73"/>
@@ -4154,21 +4196,23 @@
       <c r="I70" s="76"/>
       <c r="J70" s="76"/>
       <c r="K70" s="76"/>
-      <c r="L70" s="73"/>
-      <c r="M70" s="73"/>
-      <c r="N70" s="128"/>
+      <c r="L70" s="185"/>
+      <c r="M70" s="185"/>
+      <c r="N70" s="186"/>
       <c r="O70" s="128"/>
       <c r="P70" s="128"/>
       <c r="Q70" s="128"/>
       <c r="R70" s="128"/>
       <c r="S70" s="73"/>
-      <c r="T70" s="73"/>
+      <c r="T70" s="76"/>
       <c r="U70" s="76"/>
       <c r="V70" s="76"/>
       <c r="W70" s="76"/>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A71" s="75"/>
+    <row r="71" spans="1:44" ht="15" x14ac:dyDescent="0.15">
+      <c r="A71" s="75" t="s">
+        <v>165</v>
+      </c>
       <c r="B71" s="140"/>
       <c r="C71" s="73"/>
       <c r="D71" s="73"/>
@@ -4181,9 +4225,9 @@
       <c r="K71" s="76"/>
       <c r="L71" s="73"/>
       <c r="M71" s="73"/>
-      <c r="N71" s="128"/>
-      <c r="O71" s="128"/>
-      <c r="P71" s="128"/>
+      <c r="N71" s="186"/>
+      <c r="O71" s="186"/>
+      <c r="P71" s="186"/>
       <c r="Q71" s="128"/>
       <c r="R71" s="128"/>
       <c r="S71" s="73"/>
@@ -4192,8 +4236,10 @@
       <c r="V71" s="76"/>
       <c r="W71" s="76"/>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A72" s="75"/>
+    <row r="72" spans="1:44" ht="15" x14ac:dyDescent="0.15">
+      <c r="A72" s="75" t="s">
+        <v>164</v>
+      </c>
       <c r="B72" s="140"/>
       <c r="C72" s="73"/>
       <c r="D72" s="73"/>
@@ -4202,22 +4248,22 @@
       <c r="G72" s="76"/>
       <c r="H72" s="76"/>
       <c r="I72" s="76"/>
-      <c r="J72" s="73"/>
-      <c r="K72" s="73"/>
+      <c r="J72" s="76"/>
+      <c r="K72" s="76"/>
       <c r="L72" s="73"/>
       <c r="M72" s="73"/>
       <c r="N72" s="128"/>
       <c r="O72" s="128"/>
-      <c r="P72" s="128"/>
-      <c r="Q72" s="128"/>
-      <c r="R72" s="128"/>
+      <c r="P72" s="186"/>
+      <c r="Q72" s="186"/>
+      <c r="R72" s="186"/>
       <c r="S72" s="73"/>
       <c r="T72" s="73"/>
       <c r="U72" s="76"/>
       <c r="V72" s="76"/>
       <c r="W72" s="76"/>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A73" s="75"/>
       <c r="B73" s="140"/>
       <c r="C73" s="73"/>
@@ -4227,8 +4273,8 @@
       <c r="G73" s="76"/>
       <c r="H73" s="76"/>
       <c r="I73" s="76"/>
-      <c r="J73" s="76"/>
-      <c r="K73" s="76"/>
+      <c r="J73" s="73"/>
+      <c r="K73" s="73"/>
       <c r="L73" s="73"/>
       <c r="M73" s="73"/>
       <c r="N73" s="128"/>
@@ -4242,9 +4288,9 @@
       <c r="V73" s="76"/>
       <c r="W73" s="76"/>
     </row>
-    <row r="74" spans="1:44" s="84" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="72"/>
-      <c r="B74" s="139"/>
+    <row r="74" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A74" s="75"/>
+      <c r="B74" s="140"/>
       <c r="C74" s="73"/>
       <c r="D74" s="73"/>
       <c r="E74" s="73"/>
@@ -4252,8 +4298,8 @@
       <c r="G74" s="76"/>
       <c r="H74" s="76"/>
       <c r="I74" s="76"/>
-      <c r="J74" s="73"/>
-      <c r="K74" s="73"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
       <c r="L74" s="73"/>
       <c r="M74" s="73"/>
       <c r="N74" s="128"/>
@@ -4262,35 +4308,14 @@
       <c r="Q74" s="128"/>
       <c r="R74" s="128"/>
       <c r="S74" s="73"/>
-      <c r="T74" s="76"/>
+      <c r="T74" s="73"/>
       <c r="U74" s="76"/>
       <c r="V74" s="76"/>
       <c r="W74" s="76"/>
-      <c r="X74" s="61"/>
-      <c r="Y74" s="61"/>
-      <c r="Z74" s="61"/>
-      <c r="AA74" s="61"/>
-      <c r="AB74" s="61"/>
-      <c r="AC74" s="61"/>
-      <c r="AD74" s="61"/>
-      <c r="AE74" s="61"/>
-      <c r="AF74" s="61"/>
-      <c r="AG74" s="61"/>
-      <c r="AH74" s="61"/>
-      <c r="AI74" s="61"/>
-      <c r="AJ74" s="61"/>
-      <c r="AK74" s="61"/>
-      <c r="AL74" s="61"/>
-      <c r="AM74" s="61"/>
-      <c r="AN74" s="61"/>
-      <c r="AO74" s="61"/>
-      <c r="AP74" s="61"/>
-      <c r="AQ74" s="61"/>
-      <c r="AR74" s="61"/>
-    </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A75" s="75"/>
-      <c r="B75" s="140"/>
+    </row>
+    <row r="75" spans="1:44" s="84" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="72"/>
+      <c r="B75" s="139"/>
       <c r="C75" s="73"/>
       <c r="D75" s="73"/>
       <c r="E75" s="73"/>
@@ -4298,8 +4323,8 @@
       <c r="G75" s="76"/>
       <c r="H75" s="76"/>
       <c r="I75" s="76"/>
-      <c r="J75" s="76"/>
-      <c r="K75" s="76"/>
+      <c r="J75" s="73"/>
+      <c r="K75" s="73"/>
       <c r="L75" s="73"/>
       <c r="M75" s="73"/>
       <c r="N75" s="128"/>
@@ -4308,12 +4333,33 @@
       <c r="Q75" s="128"/>
       <c r="R75" s="128"/>
       <c r="S75" s="73"/>
-      <c r="T75" s="73"/>
-      <c r="U75" s="73"/>
-      <c r="V75" s="73"/>
-      <c r="W75" s="73"/>
-    </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="T75" s="76"/>
+      <c r="U75" s="76"/>
+      <c r="V75" s="76"/>
+      <c r="W75" s="76"/>
+      <c r="X75" s="61"/>
+      <c r="Y75" s="61"/>
+      <c r="Z75" s="61"/>
+      <c r="AA75" s="61"/>
+      <c r="AB75" s="61"/>
+      <c r="AC75" s="61"/>
+      <c r="AD75" s="61"/>
+      <c r="AE75" s="61"/>
+      <c r="AF75" s="61"/>
+      <c r="AG75" s="61"/>
+      <c r="AH75" s="61"/>
+      <c r="AI75" s="61"/>
+      <c r="AJ75" s="61"/>
+      <c r="AK75" s="61"/>
+      <c r="AL75" s="61"/>
+      <c r="AM75" s="61"/>
+      <c r="AN75" s="61"/>
+      <c r="AO75" s="61"/>
+      <c r="AP75" s="61"/>
+      <c r="AQ75" s="61"/>
+      <c r="AR75" s="61"/>
+    </row>
+    <row r="76" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A76" s="75"/>
       <c r="B76" s="140"/>
       <c r="C76" s="73"/>
@@ -4334,11 +4380,11 @@
       <c r="R76" s="128"/>
       <c r="S76" s="73"/>
       <c r="T76" s="73"/>
-      <c r="U76" s="76"/>
-      <c r="V76" s="76"/>
-      <c r="W76" s="76"/>
-    </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="U76" s="73"/>
+      <c r="V76" s="73"/>
+      <c r="W76" s="73"/>
+    </row>
+    <row r="77" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A77" s="75"/>
       <c r="B77" s="140"/>
       <c r="C77" s="73"/>
@@ -4359,111 +4405,86 @@
       <c r="R77" s="128"/>
       <c r="S77" s="73"/>
       <c r="T77" s="73"/>
-      <c r="U77" s="73"/>
-      <c r="V77" s="73"/>
-      <c r="W77" s="73"/>
-    </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A78" s="161"/>
-      <c r="B78" s="162"/>
-      <c r="C78" s="162"/>
-      <c r="D78" s="162"/>
-      <c r="E78" s="162"/>
-      <c r="F78" s="162"/>
-      <c r="G78" s="162"/>
-      <c r="H78" s="162"/>
-      <c r="I78" s="162"/>
-      <c r="J78" s="162"/>
-      <c r="K78" s="162"/>
-      <c r="L78" s="162"/>
-      <c r="M78" s="162"/>
-      <c r="N78" s="162"/>
-      <c r="O78" s="162"/>
-      <c r="P78" s="162"/>
-      <c r="Q78" s="162"/>
-      <c r="R78" s="162"/>
-      <c r="S78" s="162"/>
-      <c r="T78" s="162"/>
-      <c r="U78" s="162"/>
-      <c r="V78" s="162"/>
-      <c r="W78" s="162"/>
-    </row>
-    <row r="79" spans="1:44" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="112" t="s">
+      <c r="U77" s="76"/>
+      <c r="V77" s="76"/>
+      <c r="W77" s="76"/>
+    </row>
+    <row r="78" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A78" s="75"/>
+      <c r="B78" s="140"/>
+      <c r="C78" s="73"/>
+      <c r="D78" s="73"/>
+      <c r="E78" s="73"/>
+      <c r="F78" s="76"/>
+      <c r="G78" s="76"/>
+      <c r="H78" s="76"/>
+      <c r="I78" s="76"/>
+      <c r="J78" s="76"/>
+      <c r="K78" s="76"/>
+      <c r="L78" s="73"/>
+      <c r="M78" s="73"/>
+      <c r="N78" s="128"/>
+      <c r="O78" s="128"/>
+      <c r="P78" s="128"/>
+      <c r="Q78" s="128"/>
+      <c r="R78" s="128"/>
+      <c r="S78" s="73"/>
+      <c r="T78" s="73"/>
+      <c r="U78" s="73"/>
+      <c r="V78" s="73"/>
+      <c r="W78" s="73"/>
+    </row>
+    <row r="79" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A79" s="168"/>
+      <c r="B79" s="169"/>
+      <c r="C79" s="169"/>
+      <c r="D79" s="169"/>
+      <c r="E79" s="169"/>
+      <c r="F79" s="169"/>
+      <c r="G79" s="169"/>
+      <c r="H79" s="169"/>
+      <c r="I79" s="169"/>
+      <c r="J79" s="169"/>
+      <c r="K79" s="169"/>
+      <c r="L79" s="169"/>
+      <c r="M79" s="169"/>
+      <c r="N79" s="169"/>
+      <c r="O79" s="169"/>
+      <c r="P79" s="169"/>
+      <c r="Q79" s="169"/>
+      <c r="R79" s="169"/>
+      <c r="S79" s="169"/>
+      <c r="T79" s="169"/>
+      <c r="U79" s="169"/>
+      <c r="V79" s="169"/>
+      <c r="W79" s="169"/>
+    </row>
+    <row r="80" spans="1:44" s="99" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="112" t="s">
         <v>118</v>
       </c>
-      <c r="B79" s="147"/>
-      <c r="C79" s="113"/>
-      <c r="D79" s="113"/>
-      <c r="E79" s="113"/>
-      <c r="F79" s="113"/>
-      <c r="G79" s="113"/>
-      <c r="H79" s="113"/>
-      <c r="I79" s="113"/>
-      <c r="J79" s="113"/>
-      <c r="K79" s="113"/>
-      <c r="L79" s="113"/>
-      <c r="M79" s="113"/>
-      <c r="N79" s="113"/>
-      <c r="O79" s="113"/>
-      <c r="P79" s="113"/>
-      <c r="Q79" s="113"/>
-      <c r="R79" s="113"/>
-      <c r="S79" s="113"/>
-      <c r="T79" s="113"/>
-      <c r="U79" s="113"/>
-      <c r="V79" s="113"/>
-      <c r="W79" s="113"/>
-      <c r="X79" s="119"/>
-      <c r="Y79" s="119"/>
-      <c r="Z79" s="119"/>
-      <c r="AA79" s="119"/>
-      <c r="AB79" s="119"/>
-      <c r="AC79" s="119"/>
-      <c r="AD79" s="119"/>
-      <c r="AE79" s="119"/>
-      <c r="AF79" s="119"/>
-      <c r="AG79" s="119"/>
-      <c r="AH79" s="119"/>
-      <c r="AI79" s="119"/>
-      <c r="AJ79" s="119"/>
-      <c r="AK79" s="119"/>
-      <c r="AL79" s="119"/>
-      <c r="AM79" s="119"/>
-      <c r="AN79" s="119"/>
-      <c r="AO79" s="119"/>
-      <c r="AP79" s="119"/>
-      <c r="AQ79" s="119"/>
-      <c r="AR79" s="119"/>
-    </row>
-    <row r="80" spans="1:44" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="131" t="s">
-        <v>128</v>
-      </c>
-      <c r="B80" s="142" t="s">
-        <v>146</v>
-      </c>
-      <c r="C80" s="131"/>
-      <c r="D80" s="131"/>
-      <c r="E80" s="131"/>
-      <c r="F80" s="131"/>
-      <c r="G80" s="131"/>
-      <c r="H80" s="131"/>
-      <c r="I80" s="131"/>
-      <c r="J80" s="131"/>
-      <c r="K80" s="131"/>
-      <c r="L80" s="131"/>
-      <c r="M80" s="131"/>
-      <c r="N80" s="130"/>
-      <c r="O80" s="130"/>
-      <c r="P80" s="130"/>
-      <c r="Q80" s="130"/>
-      <c r="R80" s="130"/>
-      <c r="S80" s="131"/>
-      <c r="T80" s="131"/>
-      <c r="U80" s="131"/>
-      <c r="V80" s="131"/>
-      <c r="W80" s="131"/>
+      <c r="B80" s="147"/>
+      <c r="C80" s="113"/>
+      <c r="D80" s="113"/>
+      <c r="E80" s="113"/>
+      <c r="F80" s="113"/>
+      <c r="G80" s="113"/>
+      <c r="H80" s="113"/>
+      <c r="I80" s="113"/>
+      <c r="J80" s="113"/>
+      <c r="K80" s="113"/>
+      <c r="L80" s="113"/>
+      <c r="M80" s="113"/>
+      <c r="N80" s="113"/>
+      <c r="O80" s="113"/>
+      <c r="P80" s="113"/>
+      <c r="Q80" s="113"/>
+      <c r="R80" s="113"/>
+      <c r="S80" s="113"/>
+      <c r="T80" s="113"/>
+      <c r="U80" s="113"/>
+      <c r="V80" s="113"/>
+      <c r="W80" s="113"/>
       <c r="X80" s="119"/>
       <c r="Y80" s="119"/>
       <c r="Z80" s="119"/>
@@ -4486,12 +4507,12 @@
       <c r="AQ80" s="119"/>
       <c r="AR80" s="119"/>
     </row>
-    <row r="81" spans="1:44" s="99" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:44" s="99" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A81" s="131" t="s">
-        <v>129</v>
-      </c>
-      <c r="B81" s="138" t="s">
-        <v>147</v>
+        <v>128</v>
+      </c>
+      <c r="B81" s="142" t="s">
+        <v>146</v>
       </c>
       <c r="C81" s="131"/>
       <c r="D81" s="131"/>
@@ -4509,8 +4530,8 @@
       <c r="P81" s="130"/>
       <c r="Q81" s="130"/>
       <c r="R81" s="130"/>
-      <c r="S81" s="131"/>
-      <c r="T81" s="131"/>
+      <c r="S81" s="187"/>
+      <c r="T81" s="187"/>
       <c r="U81" s="131"/>
       <c r="V81" s="131"/>
       <c r="W81" s="131"/>
@@ -4536,187 +4557,212 @@
       <c r="AQ81" s="119"/>
       <c r="AR81" s="119"/>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A82" s="93" t="s">
-        <v>130</v>
+    <row r="82" spans="1:44" s="99" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="131" t="s">
+        <v>129</v>
       </c>
       <c r="B82" s="138" t="s">
         <v>147</v>
       </c>
-      <c r="C82" s="93"/>
-      <c r="D82" s="93"/>
-      <c r="E82" s="93"/>
-      <c r="F82" s="93"/>
-      <c r="G82" s="93"/>
-      <c r="H82" s="93"/>
-      <c r="I82" s="93"/>
-      <c r="J82" s="93"/>
-      <c r="K82" s="93"/>
-      <c r="L82" s="93"/>
-      <c r="M82" s="93"/>
-      <c r="N82" s="92"/>
-      <c r="O82" s="92"/>
-      <c r="P82" s="92"/>
-      <c r="Q82" s="92"/>
-      <c r="R82" s="92"/>
-      <c r="S82" s="93"/>
-      <c r="T82" s="93"/>
-      <c r="U82" s="93"/>
-      <c r="V82" s="93"/>
-      <c r="W82" s="93"/>
-    </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A83" s="168"/>
-      <c r="B83" s="169"/>
-      <c r="C83" s="169"/>
-      <c r="D83" s="169"/>
-      <c r="E83" s="169"/>
-      <c r="F83" s="169"/>
-      <c r="G83" s="169"/>
-      <c r="H83" s="169"/>
-      <c r="I83" s="169"/>
-      <c r="J83" s="169"/>
-      <c r="K83" s="169"/>
-      <c r="L83" s="169"/>
-      <c r="M83" s="169"/>
-      <c r="N83" s="169"/>
-      <c r="O83" s="169"/>
-      <c r="P83" s="169"/>
-      <c r="Q83" s="169"/>
-      <c r="R83" s="169"/>
-      <c r="S83" s="169"/>
-      <c r="T83" s="169"/>
-      <c r="U83" s="169"/>
-      <c r="V83" s="169"/>
-      <c r="W83" s="169"/>
-    </row>
-    <row r="84" spans="1:44" s="118" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="114" t="s">
+      <c r="C82" s="131"/>
+      <c r="D82" s="131"/>
+      <c r="E82" s="131"/>
+      <c r="F82" s="131"/>
+      <c r="G82" s="131"/>
+      <c r="H82" s="131"/>
+      <c r="I82" s="131"/>
+      <c r="J82" s="131"/>
+      <c r="K82" s="131"/>
+      <c r="L82" s="131"/>
+      <c r="M82" s="131"/>
+      <c r="N82" s="130"/>
+      <c r="O82" s="130"/>
+      <c r="P82" s="130"/>
+      <c r="Q82" s="130"/>
+      <c r="R82" s="187"/>
+      <c r="S82" s="187"/>
+      <c r="T82" s="131"/>
+      <c r="U82" s="131"/>
+      <c r="V82" s="131"/>
+      <c r="W82" s="131"/>
+      <c r="X82" s="119"/>
+      <c r="Y82" s="119"/>
+      <c r="Z82" s="119"/>
+      <c r="AA82" s="119"/>
+      <c r="AB82" s="119"/>
+      <c r="AC82" s="119"/>
+      <c r="AD82" s="119"/>
+      <c r="AE82" s="119"/>
+      <c r="AF82" s="119"/>
+      <c r="AG82" s="119"/>
+      <c r="AH82" s="119"/>
+      <c r="AI82" s="119"/>
+      <c r="AJ82" s="119"/>
+      <c r="AK82" s="119"/>
+      <c r="AL82" s="119"/>
+      <c r="AM82" s="119"/>
+      <c r="AN82" s="119"/>
+      <c r="AO82" s="119"/>
+      <c r="AP82" s="119"/>
+      <c r="AQ82" s="119"/>
+      <c r="AR82" s="119"/>
+    </row>
+    <row r="83" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A83" s="93" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="138" t="s">
+        <v>147</v>
+      </c>
+      <c r="C83" s="93"/>
+      <c r="D83" s="93"/>
+      <c r="E83" s="93"/>
+      <c r="F83" s="93"/>
+      <c r="G83" s="93"/>
+      <c r="H83" s="93"/>
+      <c r="I83" s="93"/>
+      <c r="J83" s="93"/>
+      <c r="K83" s="93"/>
+      <c r="L83" s="93"/>
+      <c r="M83" s="93"/>
+      <c r="N83" s="92"/>
+      <c r="O83" s="92"/>
+      <c r="P83" s="92"/>
+      <c r="Q83" s="188"/>
+      <c r="R83" s="188"/>
+      <c r="S83" s="93"/>
+      <c r="T83" s="93"/>
+      <c r="U83" s="93"/>
+      <c r="V83" s="93"/>
+      <c r="W83" s="93"/>
+    </row>
+    <row r="84" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A84" s="161"/>
+      <c r="B84" s="162"/>
+      <c r="C84" s="162"/>
+      <c r="D84" s="162"/>
+      <c r="E84" s="162"/>
+      <c r="F84" s="162"/>
+      <c r="G84" s="162"/>
+      <c r="H84" s="162"/>
+      <c r="I84" s="162"/>
+      <c r="J84" s="162"/>
+      <c r="K84" s="162"/>
+      <c r="L84" s="162"/>
+      <c r="M84" s="162"/>
+      <c r="N84" s="162"/>
+      <c r="O84" s="162"/>
+      <c r="P84" s="162"/>
+      <c r="Q84" s="162"/>
+      <c r="R84" s="162"/>
+      <c r="S84" s="162"/>
+      <c r="T84" s="162"/>
+      <c r="U84" s="162"/>
+      <c r="V84" s="162"/>
+      <c r="W84" s="162"/>
+    </row>
+    <row r="85" spans="1:44" s="118" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="114" t="s">
         <v>135</v>
       </c>
-      <c r="B84" s="148"/>
-      <c r="C84" s="115"/>
-      <c r="D84" s="115"/>
-      <c r="E84" s="115"/>
-      <c r="F84" s="116"/>
-      <c r="G84" s="116"/>
-      <c r="H84" s="116"/>
-      <c r="I84" s="116"/>
-      <c r="J84" s="116"/>
-      <c r="K84" s="116"/>
-      <c r="L84" s="116"/>
-      <c r="M84" s="116"/>
-      <c r="N84" s="116"/>
-      <c r="O84" s="116"/>
-      <c r="P84" s="116"/>
-      <c r="Q84" s="117"/>
-      <c r="R84" s="117"/>
-      <c r="S84" s="117"/>
-      <c r="T84" s="117"/>
-      <c r="U84" s="117"/>
-      <c r="V84" s="116"/>
-      <c r="W84" s="116"/>
-      <c r="X84" s="61"/>
-      <c r="Y84" s="61"/>
-      <c r="Z84" s="61"/>
-      <c r="AA84" s="61"/>
-      <c r="AB84" s="61"/>
-      <c r="AC84" s="61"/>
-      <c r="AD84" s="61"/>
-      <c r="AE84" s="61"/>
-      <c r="AF84" s="61"/>
-      <c r="AG84" s="61"/>
-      <c r="AH84" s="61"/>
-      <c r="AI84" s="61"/>
-      <c r="AJ84" s="61"/>
-      <c r="AK84" s="61"/>
-      <c r="AL84" s="61"/>
-      <c r="AM84" s="61"/>
-      <c r="AN84" s="61"/>
-      <c r="AO84" s="61"/>
-      <c r="AP84" s="61"/>
-      <c r="AQ84" s="61"/>
-      <c r="AR84" s="61"/>
-    </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A85" s="85" t="s">
+      <c r="B85" s="148"/>
+      <c r="C85" s="115"/>
+      <c r="D85" s="115"/>
+      <c r="E85" s="115"/>
+      <c r="F85" s="116"/>
+      <c r="G85" s="116"/>
+      <c r="H85" s="116"/>
+      <c r="I85" s="116"/>
+      <c r="J85" s="116"/>
+      <c r="K85" s="116"/>
+      <c r="L85" s="116"/>
+      <c r="M85" s="116"/>
+      <c r="N85" s="116"/>
+      <c r="O85" s="116"/>
+      <c r="P85" s="116"/>
+      <c r="Q85" s="117"/>
+      <c r="R85" s="117"/>
+      <c r="S85" s="117"/>
+      <c r="T85" s="117"/>
+      <c r="U85" s="117"/>
+      <c r="V85" s="116"/>
+      <c r="W85" s="116"/>
+      <c r="X85" s="61"/>
+      <c r="Y85" s="61"/>
+      <c r="Z85" s="61"/>
+      <c r="AA85" s="61"/>
+      <c r="AB85" s="61"/>
+      <c r="AC85" s="61"/>
+      <c r="AD85" s="61"/>
+      <c r="AE85" s="61"/>
+      <c r="AF85" s="61"/>
+      <c r="AG85" s="61"/>
+      <c r="AH85" s="61"/>
+      <c r="AI85" s="61"/>
+      <c r="AJ85" s="61"/>
+      <c r="AK85" s="61"/>
+      <c r="AL85" s="61"/>
+      <c r="AM85" s="61"/>
+      <c r="AN85" s="61"/>
+      <c r="AO85" s="61"/>
+      <c r="AP85" s="61"/>
+      <c r="AQ85" s="61"/>
+      <c r="AR85" s="61"/>
+    </row>
+    <row r="86" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A86" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="B85" s="63"/>
-      <c r="C85" s="132"/>
-      <c r="D85" s="132"/>
-      <c r="E85" s="132"/>
-      <c r="F85" s="132"/>
-      <c r="G85" s="132"/>
-      <c r="H85" s="132"/>
-      <c r="I85" s="132"/>
-      <c r="J85" s="132"/>
-      <c r="K85" s="132"/>
-      <c r="L85" s="132"/>
-      <c r="M85" s="132"/>
-      <c r="N85" s="133"/>
-      <c r="O85" s="133"/>
-      <c r="P85" s="133"/>
-      <c r="Q85" s="133"/>
-      <c r="R85" s="133"/>
-      <c r="S85" s="132"/>
-      <c r="T85" s="132"/>
-      <c r="U85" s="132"/>
-      <c r="V85" s="132"/>
-      <c r="W85" s="132"/>
-    </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A89" s="163"/>
-      <c r="B89" s="163"/>
-      <c r="C89" s="163"/>
-      <c r="D89" s="163"/>
-      <c r="E89" s="163"/>
-      <c r="F89" s="163"/>
-      <c r="G89" s="163"/>
-      <c r="H89" s="163"/>
-      <c r="I89" s="163"/>
-      <c r="J89" s="163"/>
-      <c r="K89" s="163"/>
-      <c r="L89" s="163"/>
-      <c r="M89" s="163"/>
-      <c r="N89" s="163"/>
-      <c r="O89" s="163"/>
-      <c r="P89" s="163"/>
-      <c r="Q89" s="163"/>
-      <c r="R89" s="163"/>
-      <c r="S89" s="163"/>
-      <c r="T89" s="163"/>
-      <c r="U89" s="163"/>
-      <c r="V89" s="163"/>
-      <c r="W89" s="163"/>
-    </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A90" s="164"/>
-      <c r="B90" s="156"/>
-      <c r="C90" s="156"/>
-      <c r="D90" s="156"/>
-      <c r="E90" s="156"/>
-      <c r="F90" s="156"/>
-      <c r="G90" s="156"/>
-      <c r="H90" s="156"/>
-      <c r="I90" s="156"/>
-      <c r="J90" s="156"/>
-      <c r="K90" s="156"/>
-      <c r="L90" s="156"/>
-      <c r="M90" s="156"/>
-      <c r="N90" s="156"/>
-      <c r="O90" s="156"/>
-      <c r="P90" s="156"/>
-      <c r="Q90" s="156"/>
-      <c r="R90" s="156"/>
-      <c r="S90" s="156"/>
-      <c r="T90" s="156"/>
-      <c r="U90" s="156"/>
-      <c r="V90" s="156"/>
-      <c r="W90" s="156"/>
-    </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A91" s="156"/>
+      <c r="B86" s="63"/>
+      <c r="C86" s="132"/>
+      <c r="D86" s="132"/>
+      <c r="E86" s="132"/>
+      <c r="F86" s="132"/>
+      <c r="G86" s="132"/>
+      <c r="H86" s="132"/>
+      <c r="I86" s="132"/>
+      <c r="J86" s="132"/>
+      <c r="K86" s="132"/>
+      <c r="L86" s="132"/>
+      <c r="M86" s="132"/>
+      <c r="N86" s="133"/>
+      <c r="O86" s="133"/>
+      <c r="P86" s="133"/>
+      <c r="Q86" s="133"/>
+      <c r="R86" s="133"/>
+      <c r="S86" s="132"/>
+      <c r="T86" s="132"/>
+      <c r="U86" s="132"/>
+      <c r="V86" s="132"/>
+      <c r="W86" s="132"/>
+    </row>
+    <row r="90" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A90" s="170"/>
+      <c r="B90" s="170"/>
+      <c r="C90" s="170"/>
+      <c r="D90" s="170"/>
+      <c r="E90" s="170"/>
+      <c r="F90" s="170"/>
+      <c r="G90" s="170"/>
+      <c r="H90" s="170"/>
+      <c r="I90" s="170"/>
+      <c r="J90" s="170"/>
+      <c r="K90" s="170"/>
+      <c r="L90" s="170"/>
+      <c r="M90" s="170"/>
+      <c r="N90" s="170"/>
+      <c r="O90" s="170"/>
+      <c r="P90" s="170"/>
+      <c r="Q90" s="170"/>
+      <c r="R90" s="170"/>
+      <c r="S90" s="170"/>
+      <c r="T90" s="170"/>
+      <c r="U90" s="170"/>
+      <c r="V90" s="170"/>
+      <c r="W90" s="170"/>
+    </row>
+    <row r="91" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A91" s="157"/>
       <c r="B91" s="156"/>
       <c r="C91" s="156"/>
       <c r="D91" s="156"/>
@@ -4740,23 +4786,48 @@
       <c r="V91" s="156"/>
       <c r="W91" s="156"/>
     </row>
+    <row r="92" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A92" s="156"/>
+      <c r="B92" s="156"/>
+      <c r="C92" s="156"/>
+      <c r="D92" s="156"/>
+      <c r="E92" s="156"/>
+      <c r="F92" s="156"/>
+      <c r="G92" s="156"/>
+      <c r="H92" s="156"/>
+      <c r="I92" s="156"/>
+      <c r="J92" s="156"/>
+      <c r="K92" s="156"/>
+      <c r="L92" s="156"/>
+      <c r="M92" s="156"/>
+      <c r="N92" s="156"/>
+      <c r="O92" s="156"/>
+      <c r="P92" s="156"/>
+      <c r="Q92" s="156"/>
+      <c r="R92" s="156"/>
+      <c r="S92" s="156"/>
+      <c r="T92" s="156"/>
+      <c r="U92" s="156"/>
+      <c r="V92" s="156"/>
+      <c r="W92" s="156"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A90:W90"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="C2:W2"/>
-    <mergeCell ref="A83:W83"/>
-    <mergeCell ref="A62:W62"/>
-    <mergeCell ref="B1:B6"/>
-    <mergeCell ref="A91:W91"/>
+    <mergeCell ref="A92:W92"/>
     <mergeCell ref="A7:W7"/>
     <mergeCell ref="A19:W19"/>
     <mergeCell ref="A21:W21"/>
     <mergeCell ref="A38:W38"/>
     <mergeCell ref="A49:W49"/>
-    <mergeCell ref="A78:W78"/>
-    <mergeCell ref="A89:W89"/>
+    <mergeCell ref="A79:W79"/>
+    <mergeCell ref="A90:W90"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A91:W91"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="C2:W2"/>
+    <mergeCell ref="A84:W84"/>
+    <mergeCell ref="A63:W63"/>
+    <mergeCell ref="B1:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="A46:B46">
     <cfRule type="colorScale" priority="54">
@@ -4830,7 +4901,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65:B66">
+  <conditionalFormatting sqref="A66:B67">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -4842,7 +4913,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A67:B67">
+  <conditionalFormatting sqref="A68:B68">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -4854,7 +4925,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A69:B69">
+  <conditionalFormatting sqref="A70:B70">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -4866,7 +4937,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71:B71">
+  <conditionalFormatting sqref="A72:B72">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -4878,7 +4949,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A73:B73">
+  <conditionalFormatting sqref="A74:B74">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -4890,7 +4961,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A77:B77">
+  <conditionalFormatting sqref="A78:B78">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -4902,7 +4973,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A74:B74">
+  <conditionalFormatting sqref="A75:B75">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -4926,7 +4997,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70:B70">
+  <conditionalFormatting sqref="A71:B71">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4938,7 +5009,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A76:B76">
+  <conditionalFormatting sqref="A77:B77">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4975,18 +5046,18 @@
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="43.296875" customWidth="1"/>
-    <col min="3" max="3" width="19.69921875" customWidth="1"/>
-    <col min="5" max="5" width="20.19921875" customWidth="1"/>
-    <col min="6" max="6" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.69921875" customWidth="1"/>
-    <col min="9" max="9" width="6.796875" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="171" t="s">
         <v>73</v>
       </c>
@@ -4995,7 +5066,7 @@
       <c r="E2" s="178"/>
       <c r="F2" s="178"/>
     </row>
-    <row r="3" spans="2:6" ht="21.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="171"/>
       <c r="C3" s="172" t="s">
         <v>74</v>
@@ -5006,7 +5077,7 @@
       </c>
       <c r="F3" s="173"/>
     </row>
-    <row r="4" spans="2:6" s="42" customFormat="1" ht="21.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" s="42" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="43" t="s">
         <v>3</v>
       </c>
@@ -5023,14 +5094,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="45"/>
       <c r="C5" s="56"/>
       <c r="D5" s="56"/>
       <c r="E5" s="53"/>
       <c r="F5" s="40"/>
     </row>
-    <row r="6" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
@@ -5051,7 +5122,7 @@
         <v>8.2982791586998079</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
@@ -5071,7 +5142,7 @@
         <v>1.6061185468451242</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
@@ -5091,7 +5162,7 @@
         <v>2.4091778202676863</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -5111,7 +5182,7 @@
         <v>2.6768642447418736</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
@@ -5131,7 +5202,7 @@
         <v>0.66921606118546839</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
@@ -5151,14 +5222,14 @@
         <v>0.93690248565965584</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
       <c r="E12" s="52"/>
       <c r="F12" s="54"/>
     </row>
-    <row r="13" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
@@ -5179,7 +5250,7 @@
         <v>6.8833652007648185</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
@@ -5200,7 +5271,7 @@
         <v>1.9120458891013383</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
         <v>13</v>
       </c>
@@ -5220,7 +5291,7 @@
         <v>0.38240917782026768</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>14</v>
       </c>
@@ -5240,7 +5311,7 @@
         <v>1.5296367112810707</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>15</v>
       </c>
@@ -5261,7 +5332,7 @@
         <v>1.9120458891013383</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
@@ -5281,7 +5352,7 @@
         <v>0.38240917782026768</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
@@ -5301,7 +5372,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>18</v>
       </c>
@@ -5321,7 +5392,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>19</v>
       </c>
@@ -5342,7 +5413,7 @@
         <v>1.9120458891013383</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>20</v>
       </c>
@@ -5362,7 +5433,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>21</v>
       </c>
@@ -5382,7 +5453,7 @@
         <v>1.1472275334608031</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>22</v>
       </c>
@@ -5403,7 +5474,7 @@
         <v>1.1472275334608031</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
         <v>23</v>
       </c>
@@ -5423,14 +5494,14 @@
         <v>1.1472275334608031</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="26"/>
       <c r="D26" s="26"/>
       <c r="E26" s="58"/>
       <c r="F26" s="54"/>
     </row>
-    <row r="27" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="12" t="s">
         <v>24</v>
       </c>
@@ -5451,7 +5522,7 @@
         <v>15.678776290630974</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>25</v>
       </c>
@@ -5472,7 +5543,7 @@
         <v>4.5889101338432123</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>26</v>
       </c>
@@ -5492,7 +5563,7 @@
         <v>1.5296367112810707</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="7" t="s">
         <v>27</v>
       </c>
@@ -5512,7 +5583,7 @@
         <v>3.0592734225621414</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="8" t="s">
         <v>28</v>
       </c>
@@ -5533,7 +5604,7 @@
         <v>4.9713193116634802</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7" t="s">
         <v>29</v>
       </c>
@@ -5553,7 +5624,7 @@
         <v>1.1472275334608031</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="7" t="s">
         <v>30</v>
       </c>
@@ -5573,7 +5644,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="7" t="s">
         <v>78</v>
       </c>
@@ -5593,7 +5664,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="7" t="s">
         <v>31</v>
       </c>
@@ -5613,7 +5684,7 @@
         <v>2.2944550669216062</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="8" t="s">
         <v>32</v>
       </c>
@@ -5634,7 +5705,7 @@
         <v>2.2944550669216062</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>33</v>
       </c>
@@ -5654,7 +5725,7 @@
         <v>1.1472275334608031</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="7" t="s">
         <v>79</v>
       </c>
@@ -5674,7 +5745,7 @@
         <v>1.1472275334608031</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="8" t="s">
         <v>34</v>
       </c>
@@ -5695,7 +5766,7 @@
         <v>3.8240917782026767</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="7" t="s">
         <v>35</v>
       </c>
@@ -5715,7 +5786,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="7" t="s">
         <v>36</v>
       </c>
@@ -5735,14 +5806,14 @@
         <v>3.0592734225621414</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
       <c r="F42" s="28"/>
     </row>
-    <row r="43" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="13" t="s">
         <v>37</v>
       </c>
@@ -5763,7 +5834,7 @@
         <v>43.977055449330784</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="8" t="s">
         <v>38</v>
       </c>
@@ -5784,7 +5855,7 @@
         <v>9.1778202676864247</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="7" t="s">
         <v>39</v>
       </c>
@@ -5804,7 +5875,7 @@
         <v>3.8240917782026767</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="7" t="s">
         <v>40</v>
       </c>
@@ -5824,7 +5895,7 @@
         <v>5.3537284894837471</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="8" t="s">
         <v>41</v>
       </c>
@@ -5845,7 +5916,7 @@
         <v>12.619502868068833</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
         <v>42</v>
       </c>
@@ -5865,7 +5936,7 @@
         <v>3.4416826003824093</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>43</v>
       </c>
@@ -5885,7 +5956,7 @@
         <v>4.5889101338432123</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>44</v>
       </c>
@@ -5905,7 +5976,7 @@
         <v>4.5889101338432123</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="8" t="s">
         <v>45</v>
       </c>
@@ -5926,7 +5997,7 @@
         <v>6.1185468451242828</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>46</v>
       </c>
@@ -5946,7 +6017,7 @@
         <v>3.0592734225621414</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="7" t="s">
         <v>47</v>
       </c>
@@ -5966,7 +6037,7 @@
         <v>3.0592734225621414</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="8" t="s">
         <v>48</v>
       </c>
@@ -5987,7 +6058,7 @@
         <v>16.061185468451242</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="7" t="s">
         <v>49</v>
       </c>
@@ -6007,7 +6078,7 @@
         <v>5.3537284894837471</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="7" t="s">
         <v>50</v>
       </c>
@@ -6027,7 +6098,7 @@
         <v>6.1185468451242828</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="7" t="s">
         <v>51</v>
       </c>
@@ -6047,14 +6118,14 @@
         <v>4.5889101338432123</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="59"/>
       <c r="C58" s="60"/>
       <c r="D58" s="2"/>
       <c r="E58" s="60"/>
       <c r="F58" s="29"/>
     </row>
-    <row r="59" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="10" t="s">
         <v>52</v>
       </c>
@@ -6075,7 +6146,7 @@
         <v>14.531548757170171</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="8" t="s">
         <v>53</v>
       </c>
@@ -6096,7 +6167,7 @@
         <v>2.6768642447418736</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
         <v>54</v>
       </c>
@@ -6116,7 +6187,7 @@
         <v>2.6768642447418736</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="8" t="s">
         <v>55</v>
       </c>
@@ -6137,7 +6208,7 @@
         <v>3.8240917782026767</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="7" t="s">
         <v>56</v>
       </c>
@@ -6157,7 +6228,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="7" t="s">
         <v>80</v>
       </c>
@@ -6177,7 +6248,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="7" t="s">
         <v>57</v>
       </c>
@@ -6197,7 +6268,7 @@
         <v>2.2944550669216062</v>
       </c>
     </row>
-    <row r="66" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="8" t="s">
         <v>58</v>
       </c>
@@ -6218,7 +6289,7 @@
         <v>3.0592734225621414</v>
       </c>
     </row>
-    <row r="67" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="7" t="s">
         <v>59</v>
       </c>
@@ -6238,7 +6309,7 @@
         <v>1.5296367112810707</v>
       </c>
     </row>
-    <row r="68" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="7" t="s">
         <v>60</v>
       </c>
@@ -6258,7 +6329,7 @@
         <v>1.5296367112810707</v>
       </c>
     </row>
-    <row r="69" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="8" t="s">
         <v>61</v>
       </c>
@@ -6279,7 +6350,7 @@
         <v>4.9713193116634802</v>
       </c>
     </row>
-    <row r="70" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="7" t="s">
         <v>62</v>
       </c>
@@ -6299,14 +6370,14 @@
         <v>4.9713193116634802</v>
       </c>
     </row>
-    <row r="71" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="3"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="29"/>
     </row>
-    <row r="72" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="48" t="s">
         <v>63</v>
       </c>
@@ -6327,7 +6398,7 @@
         <v>10.630975143403441</v>
       </c>
     </row>
-    <row r="73" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="8" t="s">
         <v>64</v>
       </c>
@@ -6348,7 +6419,7 @@
         <v>2.1414913957934991</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="7" t="s">
         <v>65</v>
       </c>
@@ -6368,7 +6439,7 @@
         <v>0.9177820267686424</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="7" t="s">
         <v>81</v>
       </c>
@@ -6388,7 +6459,7 @@
         <v>0.4588910133843212</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="7" t="s">
         <v>66</v>
       </c>
@@ -6408,7 +6479,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="8" t="s">
         <v>67</v>
       </c>
@@ -6428,7 +6499,7 @@
         <v>2.6768642447418736</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B78" s="8" t="s">
         <v>68</v>
       </c>
@@ -6448,7 +6519,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="79" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="8" t="s">
         <v>69</v>
       </c>
@@ -6468,7 +6539,7 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="8" t="s">
         <v>70</v>
       </c>
@@ -6488,7 +6559,7 @@
         <v>3.5181644359464626</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B81" s="8" t="s">
         <v>71</v>
       </c>
@@ -6508,14 +6579,14 @@
         <v>0.76481835564053535</v>
       </c>
     </row>
-    <row r="82" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="55"/>
       <c r="C82" s="26"/>
       <c r="D82" s="26"/>
       <c r="E82" s="26"/>
       <c r="F82" s="54"/>
     </row>
-    <row r="83" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>72</v>
       </c>
@@ -6535,21 +6606,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B84" s="179"/>
       <c r="C84" s="179"/>
       <c r="D84" s="179"/>
       <c r="E84" s="179"/>
       <c r="F84" s="179"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B85" s="178"/>
       <c r="C85" s="178"/>
       <c r="D85" s="178"/>
       <c r="E85" s="180"/>
       <c r="F85" s="180"/>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B86" s="174" t="s">
         <v>82</v>
       </c>
@@ -6558,7 +6629,7 @@
       <c r="E86" s="180"/>
       <c r="F86" s="180"/>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="s">
         <v>83</v>
       </c>
@@ -6571,7 +6642,7 @@
       <c r="E87" s="180"/>
       <c r="F87" s="180"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="s">
         <v>85</v>
       </c>
@@ -7068,6 +7139,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument Projektgruppe" ma:contentTypeID="0x0101001BCAAA424C4FC643A41D277282D4C6DA00147A2F50F690F64C87FE6572BCE8E7D1" ma:contentTypeVersion="7" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="4ef6f085b060a28d86f5839659710628">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ae84a682-57c0-4245-9851-92a7533be2d6" xmlns:ns3="e4c5f5f2-958c-44bd-9179-f1c43ce55659" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4beed55d63ba88c63baba0defe326347" ns2:_="" ns3:_="">
     <xsd:import namespace="ae84a682-57c0-4245-9851-92a7533be2d6"/>
@@ -7224,15 +7304,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90B28818-B76C-46BC-8AB6-BCD2AB0F7DDC}">
   <ds:schemaRefs>
@@ -7251,6 +7322,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C68EF06-77D1-4F69-9021-BB6F0CF7B5AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43E98B02-8317-42A1-B942-EB0DB152AA3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7267,12 +7346,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C68EF06-77D1-4F69-9021-BB6F0CF7B5AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Terminplan für Statusbericht angeschaut
</commit_message>
<xml_diff>
--- a/TerminplanungP2.xlsx
+++ b/TerminplanungP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\EIT\FS19\pro2E\Team 5\P2Pflichtenheft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F283A53-2EBD-4BE2-A521-491C8E9B334C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CB7068-54D3-42CB-AFE8-997BC8C1E694}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1028,10 +1028,34 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1050,18 +1074,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1072,16 +1084,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1089,55 +1101,43 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1468,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="62" workbookViewId="0">
-      <selection activeCell="W84" sqref="W84"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="62" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="13.8"/>
@@ -1489,44 +1489,44 @@
       <c r="E1" s="86"/>
     </row>
     <row r="2" spans="2:29" ht="21" customHeight="1">
-      <c r="B2" s="167"/>
-      <c r="C2" s="184" t="s">
+      <c r="B2" s="166"/>
+      <c r="C2" s="172" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="172" t="s">
         <v>46</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="181">
+      <c r="F2" s="168">
         <v>2019</v>
       </c>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182"/>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="183"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="170"/>
     </row>
     <row r="3" spans="2:29" ht="15.45" customHeight="1">
-      <c r="B3" s="167"/>
-      <c r="C3" s="184"/>
-      <c r="D3" s="184"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="172"/>
+      <c r="D3" s="172"/>
       <c r="E3" s="3" t="s">
         <v>85</v>
       </c>
@@ -1563,13 +1563,13 @@
       <c r="P3" s="3">
         <v>18</v>
       </c>
-      <c r="Q3" s="181" t="s">
+      <c r="Q3" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="R3" s="182"/>
-      <c r="S3" s="182"/>
-      <c r="T3" s="182"/>
-      <c r="U3" s="182"/>
+      <c r="R3" s="169"/>
+      <c r="S3" s="169"/>
+      <c r="T3" s="169"/>
+      <c r="U3" s="169"/>
       <c r="V3" s="4">
         <v>20</v>
       </c>
@@ -1587,9 +1587,9 @@
       </c>
     </row>
     <row r="4" spans="2:29" ht="36.6">
-      <c r="B4" s="167"/>
-      <c r="C4" s="184"/>
-      <c r="D4" s="184"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="172"/>
+      <c r="D4" s="172"/>
       <c r="E4" s="163" t="s">
         <v>86</v>
       </c>
@@ -1661,8 +1661,8 @@
       <c r="B5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="184"/>
-      <c r="D5" s="184"/>
+      <c r="C5" s="172"/>
+      <c r="D5" s="172"/>
       <c r="E5" s="86"/>
       <c r="F5" s="54"/>
       <c r="G5" s="54"/>
@@ -1688,39 +1688,39 @@
       <c r="AC5" s="5"/>
     </row>
     <row r="6" spans="2:29" ht="6" customHeight="1">
-      <c r="B6" s="168"/>
-      <c r="C6" s="168"/>
-      <c r="D6" s="168"/>
-      <c r="E6" s="168"/>
-      <c r="F6" s="168"/>
-      <c r="G6" s="168"/>
-      <c r="H6" s="168"/>
-      <c r="I6" s="168"/>
-      <c r="J6" s="168"/>
-      <c r="K6" s="168"/>
-      <c r="L6" s="168"/>
-      <c r="M6" s="168"/>
-      <c r="N6" s="168"/>
-      <c r="O6" s="168"/>
-      <c r="P6" s="168"/>
-      <c r="Q6" s="168"/>
-      <c r="R6" s="168"/>
-      <c r="S6" s="168"/>
-      <c r="T6" s="168"/>
-      <c r="U6" s="168"/>
-      <c r="V6" s="168"/>
-      <c r="W6" s="168"/>
-      <c r="X6" s="168"/>
-      <c r="Y6" s="168"/>
-      <c r="Z6" s="168"/>
+      <c r="B6" s="176"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="176"/>
+      <c r="K6" s="176"/>
+      <c r="L6" s="176"/>
+      <c r="M6" s="176"/>
+      <c r="N6" s="176"/>
+      <c r="O6" s="176"/>
+      <c r="P6" s="176"/>
+      <c r="Q6" s="176"/>
+      <c r="R6" s="176"/>
+      <c r="S6" s="176"/>
+      <c r="T6" s="176"/>
+      <c r="U6" s="176"/>
+      <c r="V6" s="176"/>
+      <c r="W6" s="176"/>
+      <c r="X6" s="176"/>
+      <c r="Y6" s="176"/>
+      <c r="Z6" s="176"/>
     </row>
     <row r="7" spans="2:29">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="177"/>
+      <c r="C7" s="174"/>
+      <c r="D7" s="174"/>
+      <c r="E7" s="175"/>
       <c r="F7" s="52" t="s">
         <v>2</v>
       </c>
@@ -1746,12 +1746,12 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="2:29" ht="14.4" customHeight="1">
-      <c r="B8" s="175" t="s">
+      <c r="B8" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="176"/>
-      <c r="D8" s="176"/>
-      <c r="E8" s="177"/>
+      <c r="C8" s="174"/>
+      <c r="D8" s="174"/>
+      <c r="E8" s="175"/>
       <c r="F8" s="2"/>
       <c r="G8" s="52" t="s">
         <v>2</v>
@@ -1777,12 +1777,12 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="2:29">
-      <c r="B9" s="175" t="s">
+      <c r="B9" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="176"/>
-      <c r="D9" s="176"/>
-      <c r="E9" s="177"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="174"/>
+      <c r="E9" s="175"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1808,12 +1808,12 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="2:29">
-      <c r="B10" s="175" t="s">
+      <c r="B10" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="176"/>
-      <c r="D10" s="176"/>
-      <c r="E10" s="177"/>
+      <c r="C10" s="174"/>
+      <c r="D10" s="174"/>
+      <c r="E10" s="175"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1870,12 +1870,12 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="2:29">
-      <c r="B12" s="178" t="s">
+      <c r="B12" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="179"/>
-      <c r="D12" s="179"/>
-      <c r="E12" s="180"/>
+      <c r="C12" s="183"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="184"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1901,12 +1901,12 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="2:29">
-      <c r="B13" s="175" t="s">
+      <c r="B13" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="176"/>
-      <c r="D13" s="176"/>
-      <c r="E13" s="177"/>
+      <c r="C13" s="174"/>
+      <c r="D13" s="174"/>
+      <c r="E13" s="175"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1931,12 +1931,12 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="2:29">
-      <c r="B14" s="175" t="s">
+      <c r="B14" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="176"/>
-      <c r="D14" s="176"/>
-      <c r="E14" s="177"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1962,12 +1962,12 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="2:29">
-      <c r="B15" s="175" t="s">
+      <c r="B15" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="176"/>
-      <c r="D15" s="176"/>
-      <c r="E15" s="177"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="175"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1993,12 +1993,12 @@
       </c>
     </row>
     <row r="16" spans="2:29">
-      <c r="B16" s="175" t="s">
+      <c r="B16" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="176"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="177"/>
+      <c r="C16" s="174"/>
+      <c r="D16" s="174"/>
+      <c r="E16" s="175"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -2024,12 +2024,12 @@
       </c>
     </row>
     <row r="17" spans="2:27">
-      <c r="B17" s="175" t="s">
+      <c r="B17" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="176"/>
-      <c r="D17" s="176"/>
-      <c r="E17" s="177"/>
+      <c r="C17" s="174"/>
+      <c r="D17" s="174"/>
+      <c r="E17" s="175"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -2091,31 +2091,31 @@
       <c r="AA19" s="113"/>
     </row>
     <row r="20" spans="2:27" ht="6" customHeight="1">
-      <c r="B20" s="169"/>
-      <c r="C20" s="170"/>
-      <c r="D20" s="170"/>
-      <c r="E20" s="170"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="170"/>
-      <c r="K20" s="170"/>
-      <c r="L20" s="170"/>
-      <c r="M20" s="170"/>
-      <c r="N20" s="170"/>
-      <c r="O20" s="170"/>
-      <c r="P20" s="170"/>
-      <c r="Q20" s="170"/>
-      <c r="R20" s="170"/>
-      <c r="S20" s="170"/>
-      <c r="T20" s="170"/>
-      <c r="U20" s="170"/>
-      <c r="V20" s="170"/>
-      <c r="W20" s="170"/>
-      <c r="X20" s="170"/>
-      <c r="Y20" s="170"/>
-      <c r="Z20" s="171"/>
+      <c r="B20" s="177"/>
+      <c r="C20" s="178"/>
+      <c r="D20" s="178"/>
+      <c r="E20" s="178"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="178"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="178"/>
+      <c r="J20" s="178"/>
+      <c r="K20" s="178"/>
+      <c r="L20" s="178"/>
+      <c r="M20" s="178"/>
+      <c r="N20" s="178"/>
+      <c r="O20" s="178"/>
+      <c r="P20" s="178"/>
+      <c r="Q20" s="178"/>
+      <c r="R20" s="178"/>
+      <c r="S20" s="178"/>
+      <c r="T20" s="178"/>
+      <c r="U20" s="178"/>
+      <c r="V20" s="178"/>
+      <c r="W20" s="178"/>
+      <c r="X20" s="178"/>
+      <c r="Y20" s="178"/>
+      <c r="Z20" s="179"/>
     </row>
     <row r="21" spans="2:27">
       <c r="B21" s="35" t="s">
@@ -2414,31 +2414,31 @@
       <c r="Z29" s="42"/>
     </row>
     <row r="30" spans="2:27" ht="6" customHeight="1">
-      <c r="B30" s="172"/>
-      <c r="C30" s="172"/>
-      <c r="D30" s="172"/>
-      <c r="E30" s="172"/>
-      <c r="F30" s="172"/>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="172"/>
-      <c r="K30" s="172"/>
-      <c r="L30" s="172"/>
-      <c r="M30" s="172"/>
-      <c r="N30" s="172"/>
-      <c r="O30" s="172"/>
-      <c r="P30" s="172"/>
-      <c r="Q30" s="172"/>
-      <c r="R30" s="172"/>
-      <c r="S30" s="172"/>
-      <c r="T30" s="172"/>
-      <c r="U30" s="172"/>
-      <c r="V30" s="172"/>
-      <c r="W30" s="172"/>
-      <c r="X30" s="172"/>
-      <c r="Y30" s="172"/>
-      <c r="Z30" s="172"/>
+      <c r="B30" s="180"/>
+      <c r="C30" s="180"/>
+      <c r="D30" s="180"/>
+      <c r="E30" s="180"/>
+      <c r="F30" s="180"/>
+      <c r="G30" s="180"/>
+      <c r="H30" s="180"/>
+      <c r="I30" s="180"/>
+      <c r="J30" s="180"/>
+      <c r="K30" s="180"/>
+      <c r="L30" s="180"/>
+      <c r="M30" s="180"/>
+      <c r="N30" s="180"/>
+      <c r="O30" s="180"/>
+      <c r="P30" s="180"/>
+      <c r="Q30" s="180"/>
+      <c r="R30" s="180"/>
+      <c r="S30" s="180"/>
+      <c r="T30" s="180"/>
+      <c r="U30" s="180"/>
+      <c r="V30" s="180"/>
+      <c r="W30" s="180"/>
+      <c r="X30" s="180"/>
+      <c r="Y30" s="180"/>
+      <c r="Z30" s="180"/>
     </row>
     <row r="31" spans="2:27">
       <c r="B31" s="24" t="s">
@@ -2758,31 +2758,31 @@
       <c r="Z40" s="5"/>
     </row>
     <row r="41" spans="2:26" ht="6" customHeight="1">
-      <c r="B41" s="172"/>
-      <c r="C41" s="172"/>
-      <c r="D41" s="172"/>
-      <c r="E41" s="172"/>
-      <c r="F41" s="172"/>
-      <c r="G41" s="172"/>
-      <c r="H41" s="172"/>
-      <c r="I41" s="172"/>
-      <c r="J41" s="172"/>
-      <c r="K41" s="172"/>
-      <c r="L41" s="172"/>
-      <c r="M41" s="172"/>
-      <c r="N41" s="172"/>
-      <c r="O41" s="172"/>
-      <c r="P41" s="172"/>
-      <c r="Q41" s="172"/>
-      <c r="R41" s="172"/>
-      <c r="S41" s="172"/>
-      <c r="T41" s="172"/>
-      <c r="U41" s="172"/>
-      <c r="V41" s="172"/>
-      <c r="W41" s="172"/>
-      <c r="X41" s="172"/>
-      <c r="Y41" s="172"/>
-      <c r="Z41" s="172"/>
+      <c r="B41" s="180"/>
+      <c r="C41" s="180"/>
+      <c r="D41" s="180"/>
+      <c r="E41" s="180"/>
+      <c r="F41" s="180"/>
+      <c r="G41" s="180"/>
+      <c r="H41" s="180"/>
+      <c r="I41" s="180"/>
+      <c r="J41" s="180"/>
+      <c r="K41" s="180"/>
+      <c r="L41" s="180"/>
+      <c r="M41" s="180"/>
+      <c r="N41" s="180"/>
+      <c r="O41" s="180"/>
+      <c r="P41" s="180"/>
+      <c r="Q41" s="180"/>
+      <c r="R41" s="180"/>
+      <c r="S41" s="180"/>
+      <c r="T41" s="180"/>
+      <c r="U41" s="180"/>
+      <c r="V41" s="180"/>
+      <c r="W41" s="180"/>
+      <c r="X41" s="180"/>
+      <c r="Y41" s="180"/>
+      <c r="Z41" s="180"/>
     </row>
     <row r="42" spans="2:26">
       <c r="B42" s="29" t="s">
@@ -3179,31 +3179,31 @@
       <c r="Z53" s="13"/>
     </row>
     <row r="54" spans="1:47" ht="6" customHeight="1">
-      <c r="B54" s="174"/>
-      <c r="C54" s="174"/>
-      <c r="D54" s="174"/>
-      <c r="E54" s="174"/>
-      <c r="F54" s="174"/>
-      <c r="G54" s="174"/>
-      <c r="H54" s="174"/>
-      <c r="I54" s="174"/>
-      <c r="J54" s="174"/>
-      <c r="K54" s="174"/>
-      <c r="L54" s="174"/>
-      <c r="M54" s="174"/>
-      <c r="N54" s="174"/>
-      <c r="O54" s="174"/>
-      <c r="P54" s="174"/>
-      <c r="Q54" s="174"/>
-      <c r="R54" s="174"/>
-      <c r="S54" s="174"/>
-      <c r="T54" s="174"/>
-      <c r="U54" s="174"/>
-      <c r="V54" s="174"/>
-      <c r="W54" s="174"/>
-      <c r="X54" s="174"/>
-      <c r="Y54" s="174"/>
-      <c r="Z54" s="174"/>
+      <c r="B54" s="171"/>
+      <c r="C54" s="171"/>
+      <c r="D54" s="171"/>
+      <c r="E54" s="171"/>
+      <c r="F54" s="171"/>
+      <c r="G54" s="171"/>
+      <c r="H54" s="171"/>
+      <c r="I54" s="171"/>
+      <c r="J54" s="171"/>
+      <c r="K54" s="171"/>
+      <c r="L54" s="171"/>
+      <c r="M54" s="171"/>
+      <c r="N54" s="171"/>
+      <c r="O54" s="171"/>
+      <c r="P54" s="171"/>
+      <c r="Q54" s="171"/>
+      <c r="R54" s="171"/>
+      <c r="S54" s="171"/>
+      <c r="T54" s="171"/>
+      <c r="U54" s="171"/>
+      <c r="V54" s="171"/>
+      <c r="W54" s="171"/>
+      <c r="X54" s="171"/>
+      <c r="Y54" s="171"/>
+      <c r="Z54" s="171"/>
     </row>
     <row r="55" spans="1:47" s="33" customFormat="1">
       <c r="A55" s="1"/>
@@ -3637,7 +3637,7 @@
       <c r="Y67" s="13"/>
       <c r="Z67" s="13"/>
     </row>
-    <row r="68" spans="1:47" ht="27.6">
+    <row r="68" spans="1:47" ht="13.8" customHeight="1">
       <c r="B68" s="23" t="s">
         <v>73</v>
       </c>
@@ -3671,31 +3671,31 @@
       <c r="Z68" s="83"/>
     </row>
     <row r="69" spans="1:47" ht="6" customHeight="1">
-      <c r="B69" s="173"/>
-      <c r="C69" s="173"/>
-      <c r="D69" s="173"/>
-      <c r="E69" s="173"/>
-      <c r="F69" s="173"/>
-      <c r="G69" s="173"/>
-      <c r="H69" s="173"/>
-      <c r="I69" s="173"/>
-      <c r="J69" s="173"/>
-      <c r="K69" s="173"/>
-      <c r="L69" s="173"/>
-      <c r="M69" s="173"/>
-      <c r="N69" s="173"/>
-      <c r="O69" s="173"/>
-      <c r="P69" s="173"/>
-      <c r="Q69" s="173"/>
-      <c r="R69" s="173"/>
-      <c r="S69" s="173"/>
-      <c r="T69" s="173"/>
-      <c r="U69" s="173"/>
-      <c r="V69" s="173"/>
-      <c r="W69" s="173"/>
-      <c r="X69" s="173"/>
-      <c r="Y69" s="173"/>
-      <c r="Z69" s="173"/>
+      <c r="B69" s="181"/>
+      <c r="C69" s="181"/>
+      <c r="D69" s="181"/>
+      <c r="E69" s="181"/>
+      <c r="F69" s="181"/>
+      <c r="G69" s="181"/>
+      <c r="H69" s="181"/>
+      <c r="I69" s="181"/>
+      <c r="J69" s="181"/>
+      <c r="K69" s="181"/>
+      <c r="L69" s="181"/>
+      <c r="M69" s="181"/>
+      <c r="N69" s="181"/>
+      <c r="O69" s="181"/>
+      <c r="P69" s="181"/>
+      <c r="Q69" s="181"/>
+      <c r="R69" s="181"/>
+      <c r="S69" s="181"/>
+      <c r="T69" s="181"/>
+      <c r="U69" s="181"/>
+      <c r="V69" s="181"/>
+      <c r="W69" s="181"/>
+      <c r="X69" s="181"/>
+      <c r="Y69" s="181"/>
+      <c r="Z69" s="181"/>
     </row>
     <row r="70" spans="1:47" s="34" customFormat="1">
       <c r="A70" s="51"/>
@@ -4209,96 +4209,88 @@
       <c r="Z81" s="124"/>
     </row>
     <row r="85" spans="2:26">
-      <c r="B85" s="174"/>
-      <c r="C85" s="174"/>
-      <c r="D85" s="174"/>
-      <c r="E85" s="174"/>
-      <c r="F85" s="174"/>
-      <c r="G85" s="174"/>
-      <c r="H85" s="174"/>
-      <c r="I85" s="174"/>
-      <c r="J85" s="174"/>
-      <c r="K85" s="174"/>
-      <c r="L85" s="174"/>
-      <c r="M85" s="174"/>
-      <c r="N85" s="174"/>
-      <c r="O85" s="174"/>
-      <c r="P85" s="174"/>
-      <c r="Q85" s="174"/>
-      <c r="R85" s="174"/>
-      <c r="S85" s="174"/>
-      <c r="T85" s="174"/>
-      <c r="U85" s="174"/>
-      <c r="V85" s="174"/>
-      <c r="W85" s="174"/>
-      <c r="X85" s="174"/>
-      <c r="Y85" s="174"/>
-      <c r="Z85" s="174"/>
+      <c r="B85" s="171"/>
+      <c r="C85" s="171"/>
+      <c r="D85" s="171"/>
+      <c r="E85" s="171"/>
+      <c r="F85" s="171"/>
+      <c r="G85" s="171"/>
+      <c r="H85" s="171"/>
+      <c r="I85" s="171"/>
+      <c r="J85" s="171"/>
+      <c r="K85" s="171"/>
+      <c r="L85" s="171"/>
+      <c r="M85" s="171"/>
+      <c r="N85" s="171"/>
+      <c r="O85" s="171"/>
+      <c r="P85" s="171"/>
+      <c r="Q85" s="171"/>
+      <c r="R85" s="171"/>
+      <c r="S85" s="171"/>
+      <c r="T85" s="171"/>
+      <c r="U85" s="171"/>
+      <c r="V85" s="171"/>
+      <c r="W85" s="171"/>
+      <c r="X85" s="171"/>
+      <c r="Y85" s="171"/>
+      <c r="Z85" s="171"/>
     </row>
     <row r="86" spans="2:26">
-      <c r="B86" s="166"/>
-      <c r="C86" s="167"/>
-      <c r="D86" s="167"/>
-      <c r="E86" s="167"/>
-      <c r="F86" s="166"/>
-      <c r="G86" s="166"/>
-      <c r="H86" s="166"/>
-      <c r="I86" s="166"/>
-      <c r="J86" s="166"/>
-      <c r="K86" s="166"/>
-      <c r="L86" s="166"/>
-      <c r="M86" s="166"/>
-      <c r="N86" s="166"/>
-      <c r="O86" s="166"/>
-      <c r="P86" s="166"/>
-      <c r="Q86" s="166"/>
-      <c r="R86" s="166"/>
-      <c r="S86" s="166"/>
-      <c r="T86" s="166"/>
-      <c r="U86" s="166"/>
-      <c r="V86" s="166"/>
-      <c r="W86" s="166"/>
-      <c r="X86" s="166"/>
-      <c r="Y86" s="166"/>
-      <c r="Z86" s="166"/>
+      <c r="B86" s="167"/>
+      <c r="C86" s="166"/>
+      <c r="D86" s="166"/>
+      <c r="E86" s="166"/>
+      <c r="F86" s="167"/>
+      <c r="G86" s="167"/>
+      <c r="H86" s="167"/>
+      <c r="I86" s="167"/>
+      <c r="J86" s="167"/>
+      <c r="K86" s="167"/>
+      <c r="L86" s="167"/>
+      <c r="M86" s="167"/>
+      <c r="N86" s="167"/>
+      <c r="O86" s="167"/>
+      <c r="P86" s="167"/>
+      <c r="Q86" s="167"/>
+      <c r="R86" s="167"/>
+      <c r="S86" s="167"/>
+      <c r="T86" s="167"/>
+      <c r="U86" s="167"/>
+      <c r="V86" s="167"/>
+      <c r="W86" s="167"/>
+      <c r="X86" s="167"/>
+      <c r="Y86" s="167"/>
+      <c r="Z86" s="167"/>
     </row>
     <row r="87" spans="2:26">
-      <c r="B87" s="166"/>
-      <c r="C87" s="167"/>
-      <c r="D87" s="167"/>
-      <c r="E87" s="167"/>
-      <c r="F87" s="166"/>
-      <c r="G87" s="166"/>
-      <c r="H87" s="166"/>
-      <c r="I87" s="166"/>
-      <c r="J87" s="166"/>
-      <c r="K87" s="166"/>
-      <c r="L87" s="166"/>
-      <c r="M87" s="166"/>
-      <c r="N87" s="166"/>
-      <c r="O87" s="166"/>
-      <c r="P87" s="166"/>
-      <c r="Q87" s="166"/>
-      <c r="R87" s="166"/>
-      <c r="S87" s="166"/>
-      <c r="T87" s="166"/>
-      <c r="U87" s="166"/>
-      <c r="V87" s="166"/>
-      <c r="W87" s="166"/>
-      <c r="X87" s="166"/>
-      <c r="Y87" s="166"/>
-      <c r="Z87" s="166"/>
+      <c r="B87" s="167"/>
+      <c r="C87" s="166"/>
+      <c r="D87" s="166"/>
+      <c r="E87" s="166"/>
+      <c r="F87" s="167"/>
+      <c r="G87" s="167"/>
+      <c r="H87" s="167"/>
+      <c r="I87" s="167"/>
+      <c r="J87" s="167"/>
+      <c r="K87" s="167"/>
+      <c r="L87" s="167"/>
+      <c r="M87" s="167"/>
+      <c r="N87" s="167"/>
+      <c r="O87" s="167"/>
+      <c r="P87" s="167"/>
+      <c r="Q87" s="167"/>
+      <c r="R87" s="167"/>
+      <c r="S87" s="167"/>
+      <c r="T87" s="167"/>
+      <c r="U87" s="167"/>
+      <c r="V87" s="167"/>
+      <c r="W87" s="167"/>
+      <c r="X87" s="167"/>
+      <c r="Y87" s="167"/>
+      <c r="Z87" s="167"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B86:Z86"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="F2:Z2"/>
-    <mergeCell ref="B54:Z54"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B87:Z87"/>
     <mergeCell ref="B6:Z6"/>
     <mergeCell ref="B20:Z20"/>
@@ -4315,6 +4307,14 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B86:Z86"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="F2:Z2"/>
+    <mergeCell ref="B54:Z54"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="B25">
     <cfRule type="colorScale" priority="40">
@@ -4409,29 +4409,29 @@
       <c r="E2" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="181">
+      <c r="F2" s="168">
         <v>2019</v>
       </c>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="182"/>
-      <c r="J2" s="182"/>
-      <c r="K2" s="182"/>
-      <c r="L2" s="182"/>
-      <c r="M2" s="182"/>
-      <c r="N2" s="182"/>
-      <c r="O2" s="182"/>
-      <c r="P2" s="182"/>
-      <c r="Q2" s="182"/>
-      <c r="R2" s="182"/>
-      <c r="S2" s="182"/>
-      <c r="T2" s="182"/>
-      <c r="U2" s="182"/>
-      <c r="V2" s="182"/>
-      <c r="W2" s="182"/>
-      <c r="X2" s="182"/>
-      <c r="Y2" s="182"/>
-      <c r="Z2" s="183"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="169"/>
+      <c r="I2" s="169"/>
+      <c r="J2" s="169"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="170"/>
     </row>
     <row r="3" spans="2:26">
       <c r="B3" s="1"/>
@@ -4472,13 +4472,13 @@
       <c r="P3" s="160">
         <v>18</v>
       </c>
-      <c r="Q3" s="181" t="s">
+      <c r="Q3" s="168" t="s">
         <v>84</v>
       </c>
-      <c r="R3" s="182"/>
-      <c r="S3" s="182"/>
-      <c r="T3" s="182"/>
-      <c r="U3" s="183"/>
+      <c r="R3" s="169"/>
+      <c r="S3" s="169"/>
+      <c r="T3" s="169"/>
+      <c r="U3" s="170"/>
       <c r="V3" s="4">
         <v>20</v>
       </c>
@@ -4618,11 +4618,11 @@
       <c r="Y6" s="146"/>
     </row>
     <row r="7" spans="2:26">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="177"/>
+      <c r="C7" s="174"/>
+      <c r="D7" s="175"/>
       <c r="E7" s="5"/>
       <c r="F7" s="52" t="s">
         <v>2</v>
@@ -4649,11 +4649,11 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="2:26">
-      <c r="B8" s="175" t="s">
+      <c r="B8" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="176"/>
-      <c r="D8" s="177"/>
+      <c r="C8" s="174"/>
+      <c r="D8" s="175"/>
       <c r="E8" s="5"/>
       <c r="F8" s="2"/>
       <c r="G8" s="52" t="s">
@@ -4680,11 +4680,11 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="2:26">
-      <c r="B9" s="175" t="s">
+      <c r="B9" s="173" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="176"/>
-      <c r="D9" s="177"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="175"/>
       <c r="E9" s="5"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -4711,11 +4711,11 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="2:26">
-      <c r="B10" s="175" t="s">
+      <c r="B10" s="173" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="176"/>
-      <c r="D10" s="177"/>
+      <c r="C10" s="174"/>
+      <c r="D10" s="175"/>
       <c r="E10" s="5"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -4742,11 +4742,11 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="2:26">
-      <c r="B11" s="175" t="s">
+      <c r="B11" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="176"/>
-      <c r="D11" s="177"/>
+      <c r="C11" s="174"/>
+      <c r="D11" s="175"/>
       <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -4773,11 +4773,11 @@
       <c r="Z11" s="3"/>
     </row>
     <row r="12" spans="2:26">
-      <c r="B12" s="178" t="s">
+      <c r="B12" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="179"/>
-      <c r="D12" s="180"/>
+      <c r="C12" s="183"/>
+      <c r="D12" s="184"/>
       <c r="E12" s="11"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -4804,11 +4804,11 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="2:26">
-      <c r="B13" s="175" t="s">
+      <c r="B13" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="176"/>
-      <c r="D13" s="177"/>
+      <c r="C13" s="174"/>
+      <c r="D13" s="175"/>
       <c r="E13" s="5"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -4835,11 +4835,11 @@
       <c r="Z13" s="3"/>
     </row>
     <row r="14" spans="2:26">
-      <c r="B14" s="175" t="s">
+      <c r="B14" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="176"/>
-      <c r="D14" s="177"/>
+      <c r="C14" s="174"/>
+      <c r="D14" s="175"/>
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -4866,11 +4866,11 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="2:26">
-      <c r="B15" s="175" t="s">
+      <c r="B15" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="176"/>
-      <c r="D15" s="177"/>
+      <c r="C15" s="174"/>
+      <c r="D15" s="175"/>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -4897,11 +4897,11 @@
       </c>
     </row>
     <row r="16" spans="2:26">
-      <c r="B16" s="175" t="s">
+      <c r="B16" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="176"/>
-      <c r="D16" s="177"/>
+      <c r="C16" s="174"/>
+      <c r="D16" s="175"/>
       <c r="E16" s="5"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -4928,11 +4928,11 @@
       </c>
     </row>
     <row r="17" spans="2:27">
-      <c r="B17" s="175" t="s">
+      <c r="B17" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="176"/>
-      <c r="D17" s="177"/>
+      <c r="C17" s="174"/>
+      <c r="D17" s="175"/>
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="3"/>
@@ -4988,13 +4988,13 @@
     </row>
     <row r="19" spans="2:27" ht="52.8" customHeight="1">
       <c r="B19" s="114"/>
-      <c r="C19" s="184" t="s">
+      <c r="C19" s="172" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="184" t="s">
+      <c r="D19" s="172" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="184"/>
+      <c r="E19" s="172"/>
       <c r="F19" s="150"/>
       <c r="G19" s="151"/>
       <c r="H19" s="151"/>
@@ -5020,9 +5020,9 @@
     </row>
     <row r="20" spans="2:27">
       <c r="B20" s="114"/>
-      <c r="C20" s="184"/>
-      <c r="D20" s="184"/>
-      <c r="E20" s="184"/>
+      <c r="C20" s="172"/>
+      <c r="D20" s="172"/>
+      <c r="E20" s="172"/>
       <c r="F20" s="114"/>
       <c r="G20" s="114"/>
       <c r="H20" s="114"/>
@@ -5049,9 +5049,9 @@
       <c r="B21" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="184"/>
-      <c r="D21" s="184"/>
-      <c r="E21" s="184"/>
+      <c r="C21" s="172"/>
+      <c r="D21" s="172"/>
+      <c r="E21" s="172"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -5106,11 +5106,11 @@
         <v>4</v>
       </c>
       <c r="C23" s="35"/>
-      <c r="D23" s="187">
+      <c r="D23" s="201">
         <f>SUM(D24:D24,D27,D28,D29,D30,D31,D25,D26)</f>
         <v>65</v>
       </c>
-      <c r="E23" s="187"/>
+      <c r="E23" s="201"/>
       <c r="F23" s="37"/>
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
@@ -5140,10 +5140,10 @@
       <c r="C24" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="188">
+      <c r="D24" s="185">
         <v>10</v>
       </c>
-      <c r="E24" s="189"/>
+      <c r="E24" s="186"/>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
@@ -5173,10 +5173,10 @@
       <c r="C25" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="188">
+      <c r="D25" s="185">
         <v>32</v>
       </c>
-      <c r="E25" s="189"/>
+      <c r="E25" s="186"/>
       <c r="F25" s="94"/>
       <c r="G25" s="94"/>
       <c r="H25" s="94"/>
@@ -5206,10 +5206,10 @@
       <c r="C26" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="188">
+      <c r="D26" s="185">
         <v>10</v>
       </c>
-      <c r="E26" s="189"/>
+      <c r="E26" s="186"/>
       <c r="F26" s="94"/>
       <c r="G26" s="94"/>
       <c r="H26" s="94"/>
@@ -5239,10 +5239,10 @@
       <c r="C27" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="188">
+      <c r="D27" s="185">
         <v>2</v>
       </c>
-      <c r="E27" s="189"/>
+      <c r="E27" s="186"/>
       <c r="F27" s="10"/>
       <c r="G27" s="40"/>
       <c r="H27" s="40"/>
@@ -5272,10 +5272,10 @@
       <c r="C28" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="188">
+      <c r="D28" s="185">
         <v>2</v>
       </c>
-      <c r="E28" s="189"/>
+      <c r="E28" s="186"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -5305,10 +5305,10 @@
       <c r="C29" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="188">
+      <c r="D29" s="185">
         <v>2</v>
       </c>
-      <c r="E29" s="189"/>
+      <c r="E29" s="186"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -5338,10 +5338,10 @@
       <c r="C30" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="188">
+      <c r="D30" s="185">
         <v>4</v>
       </c>
-      <c r="E30" s="189"/>
+      <c r="E30" s="186"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -5371,10 +5371,10 @@
       <c r="C31" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="188">
+      <c r="D31" s="185">
         <v>3</v>
       </c>
-      <c r="E31" s="189"/>
+      <c r="E31" s="186"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
@@ -5429,11 +5429,11 @@
         <v>5</v>
       </c>
       <c r="C33" s="153"/>
-      <c r="D33" s="190">
+      <c r="D33" s="202">
         <f>SUM(D39,D34)</f>
         <v>75</v>
       </c>
-      <c r="E33" s="191"/>
+      <c r="E33" s="203"/>
       <c r="F33" s="147"/>
       <c r="G33" s="147"/>
       <c r="H33" s="147"/>
@@ -5463,11 +5463,11 @@
       <c r="C34" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="185">
+      <c r="D34" s="189">
         <f>SUM(D35:E38)</f>
         <v>43</v>
       </c>
-      <c r="E34" s="186"/>
+      <c r="E34" s="190"/>
       <c r="F34" s="75"/>
       <c r="G34" s="75"/>
       <c r="H34" s="75"/>
@@ -5495,10 +5495,10 @@
         <v>50</v>
       </c>
       <c r="C35" s="70"/>
-      <c r="D35" s="185">
+      <c r="D35" s="189">
         <v>12</v>
       </c>
-      <c r="E35" s="186"/>
+      <c r="E35" s="190"/>
       <c r="F35" s="78"/>
       <c r="G35" s="78"/>
       <c r="H35" s="78"/>
@@ -5526,10 +5526,10 @@
         <v>47</v>
       </c>
       <c r="C36" s="70"/>
-      <c r="D36" s="185">
+      <c r="D36" s="189">
         <v>15</v>
       </c>
-      <c r="E36" s="186"/>
+      <c r="E36" s="190"/>
       <c r="F36" s="116"/>
       <c r="G36" s="116"/>
       <c r="H36" s="78"/>
@@ -5557,10 +5557,10 @@
         <v>48</v>
       </c>
       <c r="C37" s="70"/>
-      <c r="D37" s="185">
+      <c r="D37" s="189">
         <v>10</v>
       </c>
-      <c r="E37" s="186"/>
+      <c r="E37" s="190"/>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
       <c r="H37" s="78"/>
@@ -5588,10 +5588,10 @@
         <v>49</v>
       </c>
       <c r="C38" s="70"/>
-      <c r="D38" s="185">
+      <c r="D38" s="189">
         <v>6</v>
       </c>
-      <c r="E38" s="186"/>
+      <c r="E38" s="190"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
       <c r="H38" s="78"/>
@@ -5621,11 +5621,11 @@
       <c r="C39" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="188">
+      <c r="D39" s="185">
         <f>SUM(D40:E42)</f>
         <v>32</v>
       </c>
-      <c r="E39" s="189"/>
+      <c r="E39" s="186"/>
       <c r="F39" s="76"/>
       <c r="G39" s="76"/>
       <c r="H39" s="76"/>
@@ -5653,10 +5653,10 @@
         <v>36</v>
       </c>
       <c r="C40" s="71"/>
-      <c r="D40" s="192">
+      <c r="D40" s="197">
         <v>10</v>
       </c>
-      <c r="E40" s="193"/>
+      <c r="E40" s="198"/>
       <c r="F40" s="77"/>
       <c r="G40" s="76"/>
       <c r="H40" s="76"/>
@@ -5684,10 +5684,10 @@
         <v>40</v>
       </c>
       <c r="C41" s="68"/>
-      <c r="D41" s="192">
+      <c r="D41" s="197">
         <v>10</v>
       </c>
-      <c r="E41" s="193"/>
+      <c r="E41" s="198"/>
       <c r="F41" s="10"/>
       <c r="G41" s="78"/>
       <c r="H41" s="75"/>
@@ -5715,10 +5715,10 @@
         <v>37</v>
       </c>
       <c r="C42" s="71"/>
-      <c r="D42" s="192">
+      <c r="D42" s="197">
         <v>12</v>
       </c>
-      <c r="E42" s="193"/>
+      <c r="E42" s="198"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
@@ -5773,11 +5773,11 @@
         <v>6</v>
       </c>
       <c r="C44" s="72"/>
-      <c r="D44" s="194">
+      <c r="D44" s="199">
         <f>SUM(D45,D49,D53,D55)</f>
         <v>147</v>
       </c>
-      <c r="E44" s="195"/>
+      <c r="E44" s="200"/>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
       <c r="H44" s="30"/>
@@ -5807,11 +5807,11 @@
       <c r="C45" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D45" s="185">
+      <c r="D45" s="189">
         <f>SUM(D46:E48)</f>
         <v>45</v>
       </c>
-      <c r="E45" s="186"/>
+      <c r="E45" s="190"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
       <c r="H45" s="79"/>
@@ -5839,10 +5839,10 @@
         <v>31</v>
       </c>
       <c r="C46" s="67"/>
-      <c r="D46" s="188">
+      <c r="D46" s="185">
         <v>20</v>
       </c>
-      <c r="E46" s="189"/>
+      <c r="E46" s="186"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="79"/>
@@ -5870,10 +5870,10 @@
         <v>51</v>
       </c>
       <c r="C47" s="67"/>
-      <c r="D47" s="188">
+      <c r="D47" s="185">
         <v>15</v>
       </c>
-      <c r="E47" s="189"/>
+      <c r="E47" s="186"/>
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="79"/>
@@ -5901,10 +5901,10 @@
         <v>52</v>
       </c>
       <c r="C48" s="67"/>
-      <c r="D48" s="188">
+      <c r="D48" s="185">
         <v>10</v>
       </c>
-      <c r="E48" s="189"/>
+      <c r="E48" s="186"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
@@ -5934,11 +5934,11 @@
       <c r="C49" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="185">
+      <c r="D49" s="189">
         <f>SUM(D50:E52)</f>
         <v>40</v>
       </c>
-      <c r="E49" s="186"/>
+      <c r="E49" s="190"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
@@ -5966,10 +5966,10 @@
         <v>38</v>
       </c>
       <c r="C50" s="67"/>
-      <c r="D50" s="188">
+      <c r="D50" s="185">
         <v>18</v>
       </c>
-      <c r="E50" s="189"/>
+      <c r="E50" s="186"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
@@ -5997,10 +5997,10 @@
         <v>39</v>
       </c>
       <c r="C51" s="67"/>
-      <c r="D51" s="188">
+      <c r="D51" s="185">
         <v>12</v>
       </c>
-      <c r="E51" s="189"/>
+      <c r="E51" s="186"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
@@ -6028,10 +6028,10 @@
         <v>41</v>
       </c>
       <c r="C52" s="67"/>
-      <c r="D52" s="188">
+      <c r="D52" s="185">
         <v>10</v>
       </c>
-      <c r="E52" s="189"/>
+      <c r="E52" s="186"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
@@ -6061,11 +6061,11 @@
       <c r="C53" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D53" s="185">
+      <c r="D53" s="189">
         <f>SUM(D54:D54)</f>
         <v>10</v>
       </c>
-      <c r="E53" s="186"/>
+      <c r="E53" s="190"/>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
@@ -6093,10 +6093,10 @@
         <v>42</v>
       </c>
       <c r="C54" s="67"/>
-      <c r="D54" s="188">
+      <c r="D54" s="185">
         <v>10</v>
       </c>
-      <c r="E54" s="189"/>
+      <c r="E54" s="186"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
@@ -6124,10 +6124,10 @@
         <v>74</v>
       </c>
       <c r="C55" s="66"/>
-      <c r="D55" s="188">
+      <c r="D55" s="185">
         <v>52</v>
       </c>
-      <c r="E55" s="189"/>
+      <c r="E55" s="186"/>
       <c r="F55" s="80"/>
       <c r="G55" s="80"/>
       <c r="H55" s="80"/>
@@ -6182,11 +6182,11 @@
         <v>7</v>
       </c>
       <c r="C57" s="73"/>
-      <c r="D57" s="198">
+      <c r="D57" s="195">
         <f>SUM(D58,D66,D70)</f>
         <v>495</v>
       </c>
-      <c r="E57" s="199"/>
+      <c r="E57" s="196"/>
       <c r="F57" s="44"/>
       <c r="G57" s="44"/>
       <c r="H57" s="44"/>
@@ -6216,11 +6216,11 @@
       <c r="C58" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="185">
+      <c r="D58" s="189">
         <f>SUM(D59:E65)</f>
         <v>260</v>
       </c>
-      <c r="E58" s="186"/>
+      <c r="E58" s="190"/>
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
       <c r="H58" s="83"/>
@@ -6248,10 +6248,10 @@
         <v>53</v>
       </c>
       <c r="C59" s="70"/>
-      <c r="D59" s="185">
+      <c r="D59" s="189">
         <v>35</v>
       </c>
-      <c r="E59" s="186"/>
+      <c r="E59" s="190"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="83"/>
@@ -6279,10 +6279,10 @@
         <v>54</v>
       </c>
       <c r="C60" s="70"/>
-      <c r="D60" s="185">
+      <c r="D60" s="189">
         <v>60</v>
       </c>
-      <c r="E60" s="186"/>
+      <c r="E60" s="190"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
@@ -6310,10 +6310,10 @@
         <v>55</v>
       </c>
       <c r="C61" s="68"/>
-      <c r="D61" s="192">
+      <c r="D61" s="197">
         <v>75</v>
       </c>
-      <c r="E61" s="193"/>
+      <c r="E61" s="198"/>
       <c r="F61" s="10"/>
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
@@ -6341,10 +6341,10 @@
         <v>58</v>
       </c>
       <c r="C62" s="68"/>
-      <c r="D62" s="192">
+      <c r="D62" s="197">
         <v>30</v>
       </c>
-      <c r="E62" s="193"/>
+      <c r="E62" s="198"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
@@ -6372,10 +6372,10 @@
         <v>56</v>
       </c>
       <c r="C63" s="68"/>
-      <c r="D63" s="192">
+      <c r="D63" s="197">
         <v>30</v>
       </c>
-      <c r="E63" s="193"/>
+      <c r="E63" s="198"/>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
       <c r="H63" s="10"/>
@@ -6403,10 +6403,10 @@
         <v>57</v>
       </c>
       <c r="C64" s="68"/>
-      <c r="D64" s="192">
+      <c r="D64" s="197">
         <v>15</v>
       </c>
-      <c r="E64" s="193"/>
+      <c r="E64" s="198"/>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
@@ -6434,10 +6434,10 @@
         <v>76</v>
       </c>
       <c r="C65" s="68"/>
-      <c r="D65" s="192">
+      <c r="D65" s="197">
         <v>15</v>
       </c>
-      <c r="E65" s="193"/>
+      <c r="E65" s="198"/>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
@@ -6467,11 +6467,11 @@
       <c r="C66" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D66" s="188">
+      <c r="D66" s="185">
         <f>SUM(D67:E69)</f>
         <v>55</v>
       </c>
-      <c r="E66" s="189"/>
+      <c r="E66" s="186"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
@@ -6499,10 +6499,10 @@
         <v>43</v>
       </c>
       <c r="C67" s="68"/>
-      <c r="D67" s="192">
+      <c r="D67" s="197">
         <v>15</v>
       </c>
-      <c r="E67" s="193"/>
+      <c r="E67" s="198"/>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
       <c r="H67" s="10"/>
@@ -6530,10 +6530,10 @@
         <v>45</v>
       </c>
       <c r="C68" s="68"/>
-      <c r="D68" s="192">
+      <c r="D68" s="197">
         <v>25</v>
       </c>
-      <c r="E68" s="193"/>
+      <c r="E68" s="198"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
       <c r="H68" s="10"/>
@@ -6561,10 +6561,10 @@
         <v>44</v>
       </c>
       <c r="C69" s="68"/>
-      <c r="D69" s="192">
+      <c r="D69" s="197">
         <v>15</v>
       </c>
-      <c r="E69" s="193"/>
+      <c r="E69" s="198"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
       <c r="H69" s="10"/>
@@ -6594,10 +6594,10 @@
       <c r="C70" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="D70" s="192">
+      <c r="D70" s="197">
         <v>180</v>
       </c>
-      <c r="E70" s="193"/>
+      <c r="E70" s="198"/>
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
@@ -6652,11 +6652,11 @@
         <v>20</v>
       </c>
       <c r="C72" s="74"/>
-      <c r="D72" s="196">
+      <c r="D72" s="193">
         <f>SUM(D73:E76)</f>
         <v>192</v>
       </c>
-      <c r="E72" s="197"/>
+      <c r="E72" s="194"/>
       <c r="F72" s="48"/>
       <c r="G72" s="48"/>
       <c r="H72" s="48"/>
@@ -6686,10 +6686,10 @@
       <c r="C73" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D73" s="185">
+      <c r="D73" s="189">
         <v>60</v>
       </c>
-      <c r="E73" s="186"/>
+      <c r="E73" s="190"/>
       <c r="F73" s="63"/>
       <c r="G73" s="63"/>
       <c r="H73" s="63"/>
@@ -6719,10 +6719,10 @@
       <c r="C74" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D74" s="188">
+      <c r="D74" s="185">
         <v>40</v>
       </c>
-      <c r="E74" s="189"/>
+      <c r="E74" s="186"/>
       <c r="F74" s="63"/>
       <c r="G74" s="63"/>
       <c r="H74" s="63"/>
@@ -6752,10 +6752,10 @@
       <c r="C75" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D75" s="188">
+      <c r="D75" s="185">
         <v>50</v>
       </c>
-      <c r="E75" s="189"/>
+      <c r="E75" s="186"/>
       <c r="F75" s="63"/>
       <c r="G75" s="63"/>
       <c r="H75" s="63"/>
@@ -6785,10 +6785,10 @@
       <c r="C76" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D76" s="188">
+      <c r="D76" s="185">
         <v>42</v>
       </c>
-      <c r="E76" s="189"/>
+      <c r="E76" s="186"/>
       <c r="F76" s="63"/>
       <c r="G76" s="63"/>
       <c r="H76" s="63"/>
@@ -6843,11 +6843,11 @@
         <v>59</v>
       </c>
       <c r="C78" s="92"/>
-      <c r="D78" s="202">
+      <c r="D78" s="191">
         <f>SUM(D79:E80)</f>
         <v>24</v>
       </c>
-      <c r="E78" s="203"/>
+      <c r="E78" s="192"/>
       <c r="F78" s="93"/>
       <c r="G78" s="93"/>
       <c r="H78" s="93"/>
@@ -6877,10 +6877,10 @@
       <c r="C79" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D79" s="188">
+      <c r="D79" s="185">
         <v>6</v>
       </c>
-      <c r="E79" s="189"/>
+      <c r="E79" s="186"/>
       <c r="F79" s="28"/>
       <c r="G79" s="28"/>
       <c r="H79" s="28"/>
@@ -6910,10 +6910,10 @@
       <c r="C80" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D80" s="188">
+      <c r="D80" s="185">
         <v>18</v>
       </c>
-      <c r="E80" s="189"/>
+      <c r="E80" s="186"/>
       <c r="F80" s="28"/>
       <c r="G80" s="28"/>
       <c r="H80" s="28"/>
@@ -6968,11 +6968,11 @@
         <v>82</v>
       </c>
       <c r="C82" s="120"/>
-      <c r="D82" s="200">
+      <c r="D82" s="187">
         <f>SUM(D83)</f>
         <v>48</v>
       </c>
-      <c r="E82" s="201"/>
+      <c r="E82" s="188"/>
       <c r="F82" s="121"/>
       <c r="G82" s="121"/>
       <c r="H82" s="121"/>
@@ -7000,10 +7000,10 @@
         <v>62</v>
       </c>
       <c r="C83" s="3"/>
-      <c r="D83" s="181">
+      <c r="D83" s="168">
         <v>48</v>
       </c>
-      <c r="E83" s="183"/>
+      <c r="E83" s="170"/>
       <c r="F83" s="124"/>
       <c r="G83" s="124"/>
       <c r="H83" s="124"/>
@@ -7029,6 +7029,60 @@
     <row r="84" spans="2:26" ht="3.6" customHeight="1"/>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="F2:Z2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:E21"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
     <mergeCell ref="D80:E80"/>
     <mergeCell ref="D82:E82"/>
     <mergeCell ref="D83:E83"/>
@@ -7045,60 +7099,6 @@
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F2:Z2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:E21"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="B27:C27">
     <cfRule type="colorScale" priority="5">
@@ -7288,9 +7288,9 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="6.6" customHeight="1">
-      <c r="B12" s="172"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="172"/>
+      <c r="B12" s="180"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="180"/>
     </row>
     <row r="13" spans="2:5" ht="14.4" customHeight="1">
       <c r="B13" s="24" t="s">
@@ -7390,9 +7390,9 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="6.6" customHeight="1">
-      <c r="B23" s="172"/>
-      <c r="C23" s="172"/>
-      <c r="D23" s="172"/>
+      <c r="B23" s="180"/>
+      <c r="C23" s="180"/>
+      <c r="D23" s="180"/>
     </row>
     <row r="24" spans="2:4" ht="14.4" customHeight="1">
       <c r="B24" s="29" t="s">
@@ -7513,9 +7513,9 @@
       </c>
     </row>
     <row r="36" spans="2:4" ht="6.6" customHeight="1">
-      <c r="B36" s="172"/>
-      <c r="C36" s="172"/>
-      <c r="D36" s="172"/>
+      <c r="B36" s="180"/>
+      <c r="C36" s="180"/>
+      <c r="D36" s="180"/>
     </row>
     <row r="37" spans="2:4" ht="14.4" customHeight="1">
       <c r="B37" s="43" t="s">
@@ -8051,6 +8051,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <if6c3b60cb7946a497c90999f960d465 xmlns="ae84a682-57c0-4245-9851-92a7533be2d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </if6c3b60cb7946a497c90999f960d465>
+    <TaxCatchAll xmlns="e4c5f5f2-958c-44bd-9179-f1c43ce55659"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument Projektgruppe" ma:contentTypeID="0x0101001BCAAA424C4FC643A41D277282D4C6DA00147A2F50F690F64C87FE6572BCE8E7D1" ma:contentTypeVersion="7" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="4ef6f085b060a28d86f5839659710628">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ae84a682-57c0-4245-9851-92a7533be2d6" xmlns:ns3="e4c5f5f2-958c-44bd-9179-f1c43ce55659" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4beed55d63ba88c63baba0defe326347" ns2:_="" ns3:_="">
     <xsd:import namespace="ae84a682-57c0-4245-9851-92a7533be2d6"/>
@@ -8207,27 +8227,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90B28818-B76C-46BC-8AB6-BCD2AB0F7DDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="e4c5f5f2-958c-44bd-9179-f1c43ce55659"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ae84a682-57c0-4245-9851-92a7533be2d6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <if6c3b60cb7946a497c90999f960d465 xmlns="ae84a682-57c0-4245-9851-92a7533be2d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </if6c3b60cb7946a497c90999f960d465>
-    <TaxCatchAll xmlns="e4c5f5f2-958c-44bd-9179-f1c43ce55659"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C68EF06-77D1-4F69-9021-BB6F0CF7B5AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43E98B02-8317-42A1-B942-EB0DB152AA3D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8244,29 +8269,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C68EF06-77D1-4F69-9021-BB6F0CF7B5AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90B28818-B76C-46BC-8AB6-BCD2AB0F7DDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="e4c5f5f2-958c-44bd-9179-f1c43ce55659"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ae84a682-57c0-4245-9851-92a7533be2d6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>